<commit_message>
Abhinav | Add USC wheat data to resources
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/informationist/Projects/src/github.com/usc-isi-i2/sheet_annotator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B23CE518-68E3-0543-B692-D0CECC0E8311}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF2A525-575A-B94E-9738-AD72E9FC34B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="40" windowWidth="25440" windowHeight="15360" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
   </bookViews>
   <sheets>
     <sheet name="india_wheat" sheetId="1" r:id="rId1"/>
+    <sheet name="shifted_india_wheat" sheetId="3" r:id="rId2"/>
+    <sheet name="usa_wheat" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="84">
   <si>
     <t>Data Last Updated on:</t>
   </si>
@@ -238,6 +240,54 @@
   </si>
   <si>
     <t xml:space="preserve"> Tonnes/Ha</t>
+  </si>
+  <si>
+    <t>UNITED STATES OF AMERICA</t>
+  </si>
+  <si>
+    <t>June/May</t>
+  </si>
+  <si>
+    <t>68.08</t>
+  </si>
+  <si>
+    <t>71.30</t>
+  </si>
+  <si>
+    <t>80.14</t>
+  </si>
+  <si>
+    <t>81.21</t>
+  </si>
+  <si>
+    <t>88.06</t>
+  </si>
+  <si>
+    <t>80.81</t>
+  </si>
+  <si>
+    <t>84.89</t>
+  </si>
+  <si>
+    <t>82.34</t>
+  </si>
+  <si>
+    <t>75.33</t>
+  </si>
+  <si>
+    <t>79.66</t>
+  </si>
+  <si>
+    <t>92.60</t>
+  </si>
+  <si>
+    <t>83.80</t>
+  </si>
+  <si>
+    <t>85.14</t>
+  </si>
+  <si>
+    <t>For example, in the 2017/18 balance, the NMY refers to the crop that is harvested from June 2017 to September 2017 and marketed between June 2017 and May 2018</t>
   </si>
 </sst>
 </file>
@@ -357,7 +407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -370,9 +420,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -380,8 +427,22 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -391,9 +452,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,8 +769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E291444-CA67-AD49-A6F4-57BDC8CB34D6}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -836,187 +895,187 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K10" s="7" t="s">
+      <c r="K10" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="O10" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="8">
         <v>8.6</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="8">
         <v>10</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="8">
         <v>12</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="8">
         <v>13.43</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="8">
         <v>16.100000000000001</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="8">
         <v>17</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="8">
         <v>21</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <v>24.5</v>
       </c>
-      <c r="K11" s="9">
+      <c r="K11" s="8">
         <v>21</v>
       </c>
-      <c r="L11" s="9">
+      <c r="L11" s="8">
         <v>23</v>
       </c>
-      <c r="M11" s="9">
+      <c r="M11" s="8">
         <v>20</v>
       </c>
-      <c r="N11" s="9">
+      <c r="N11" s="8">
         <v>13.5</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="8">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="8">
         <v>69.349999999999994</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="8">
         <v>75.81</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="8">
         <v>78.569999999999993</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="8">
         <v>80.680000000000007</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="8">
         <v>80.8</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="8">
         <v>86.87</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="8">
         <v>94.88</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <v>93.51</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K12" s="8">
         <v>95.85</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L12" s="8">
         <v>86.53</v>
       </c>
-      <c r="M12" s="9">
+      <c r="M12" s="8">
         <v>92.29</v>
       </c>
-      <c r="N12" s="9">
+      <c r="N12" s="8">
         <v>98.51</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="8">
         <v>99.7</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A13" s="8" t="s">
+      <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="8">
         <v>6.11</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="8">
         <v>1.82</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="8">
         <v>0.02</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="8">
         <v>0.17</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="8">
         <v>0.19</v>
       </c>
-      <c r="H13" s="9">
-        <v>0</v>
-      </c>
-      <c r="I13" s="9">
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
         <v>0.01</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <v>0.01</v>
       </c>
-      <c r="K13" s="9">
+      <c r="K13" s="8">
         <v>0.03</v>
       </c>
-      <c r="L13" s="9">
+      <c r="L13" s="8">
         <v>0.52</v>
       </c>
-      <c r="M13" s="9">
+      <c r="M13" s="8">
         <v>5.75</v>
       </c>
-      <c r="N13" s="9">
+      <c r="N13" s="8">
         <v>1.65</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13" s="8">
         <v>0.15</v>
       </c>
     </row>
@@ -1024,328 +1083,328 @@
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G14" s="7" t="s">
+      <c r="G14" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="I14" s="7" t="s">
+      <c r="I14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="7" t="s">
+      <c r="J14" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="7" t="s">
+      <c r="L14" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="M14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="N14" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O14" s="7" t="s">
+      <c r="O14" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="8">
         <v>74.02</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="8">
         <v>75.62</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="8">
         <v>77.16</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>78.13</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="8">
         <v>80.03</v>
       </c>
-      <c r="H15" s="9">
+      <c r="H15" s="8">
         <v>82</v>
       </c>
-      <c r="I15" s="9">
+      <c r="I15" s="8">
         <v>84.59</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <v>91</v>
       </c>
-      <c r="K15" s="9">
+      <c r="K15" s="8">
         <v>90.5</v>
       </c>
-      <c r="L15" s="9">
+      <c r="L15" s="8">
         <v>89</v>
       </c>
-      <c r="M15" s="9">
+      <c r="M15" s="8">
         <v>104.1</v>
       </c>
-      <c r="N15" s="9">
+      <c r="N15" s="8">
         <v>95.15</v>
       </c>
-      <c r="O15" s="9">
+      <c r="O15" s="8">
         <v>97.25</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="11">
+      <c r="C16" s="10">
         <v>68.17</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>69.02</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>70</v>
       </c>
-      <c r="F16" s="11">
+      <c r="F16" s="10">
         <v>71</v>
       </c>
-      <c r="G16" s="11">
+      <c r="G16" s="10">
         <v>72.099999999999994</v>
       </c>
-      <c r="H16" s="11">
+      <c r="H16" s="10">
         <v>73</v>
       </c>
-      <c r="I16" s="11">
+      <c r="I16" s="10">
         <v>74.5</v>
       </c>
-      <c r="J16" s="11">
+      <c r="J16" s="10">
         <v>75.599999999999994</v>
       </c>
-      <c r="K16" s="11">
+      <c r="K16" s="10">
         <v>76.900000000000006</v>
       </c>
-      <c r="L16" s="11">
+      <c r="L16" s="10">
         <v>78.2</v>
       </c>
-      <c r="M16" s="11">
+      <c r="M16" s="10">
         <v>79.2</v>
       </c>
-      <c r="N16" s="11">
+      <c r="N16" s="10">
         <v>80.099999999999994</v>
       </c>
-      <c r="O16" s="11">
+      <c r="O16" s="10">
         <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="10">
         <v>1.43</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>1.48</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>1.52</v>
       </c>
-      <c r="F17" s="11">
+      <c r="F17" s="10">
         <v>1.6</v>
       </c>
-      <c r="G17" s="11">
+      <c r="G17" s="10">
         <v>2.5</v>
       </c>
-      <c r="H17" s="11">
+      <c r="H17" s="10">
         <v>2.5</v>
       </c>
-      <c r="I17" s="11">
+      <c r="I17" s="10">
         <v>3</v>
       </c>
-      <c r="J17" s="11">
+      <c r="J17" s="10">
         <v>4.5</v>
       </c>
-      <c r="K17" s="11">
+      <c r="K17" s="10">
         <v>5</v>
       </c>
-      <c r="L17" s="11">
+      <c r="L17" s="10">
         <v>5</v>
       </c>
-      <c r="M17" s="11">
+      <c r="M17" s="10">
         <v>5</v>
       </c>
-      <c r="N17" s="11">
+      <c r="N17" s="10">
         <v>5</v>
       </c>
-      <c r="O17" s="11">
+      <c r="O17" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="11">
+      <c r="C18" s="10">
         <v>4.42</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <v>5.12</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <v>5.64</v>
       </c>
-      <c r="F18" s="11">
+      <c r="F18" s="10">
         <v>5.53</v>
       </c>
-      <c r="G18" s="11">
+      <c r="G18" s="10">
         <v>5.43</v>
       </c>
-      <c r="H18" s="11">
+      <c r="H18" s="10">
         <v>6.5</v>
       </c>
-      <c r="I18" s="11">
+      <c r="I18" s="10">
         <v>7.09</v>
       </c>
-      <c r="J18" s="11">
+      <c r="J18" s="10">
         <v>10.9</v>
       </c>
-      <c r="K18" s="11">
+      <c r="K18" s="10">
         <v>8.6</v>
       </c>
-      <c r="L18" s="11">
+      <c r="L18" s="10">
         <v>5.8</v>
       </c>
-      <c r="M18" s="11">
+      <c r="M18" s="10">
         <v>19.899999999999999</v>
       </c>
-      <c r="N18" s="11">
+      <c r="N18" s="10">
         <v>10.050000000000001</v>
       </c>
-      <c r="O18" s="11">
+      <c r="O18" s="10">
         <v>11.25</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="8">
         <v>0.05</v>
       </c>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0</v>
-      </c>
-      <c r="F19" s="9">
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0</v>
+      </c>
+      <c r="F19" s="8">
         <v>0.05</v>
       </c>
-      <c r="G19" s="9">
+      <c r="G19" s="8">
         <v>0.06</v>
       </c>
-      <c r="H19" s="9">
+      <c r="H19" s="8">
         <v>0.87</v>
       </c>
-      <c r="I19" s="9">
+      <c r="I19" s="8">
         <v>6.8</v>
       </c>
-      <c r="J19" s="9">
+      <c r="J19" s="8">
         <v>6.03</v>
       </c>
-      <c r="K19" s="9">
+      <c r="K19" s="8">
         <v>3.38</v>
       </c>
-      <c r="L19" s="9">
+      <c r="L19" s="8">
         <v>1.06</v>
       </c>
-      <c r="M19" s="9">
+      <c r="M19" s="8">
         <v>0.44</v>
       </c>
-      <c r="N19" s="9">
+      <c r="N19" s="8">
         <v>0.51</v>
       </c>
-      <c r="O19" s="9">
+      <c r="O19" s="8">
         <v>0.6</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A20" s="8" t="s">
+      <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>10</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>12</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>13.43</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>16.100000000000001</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>17</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>21</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>24.5</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <v>21</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="8">
         <v>23</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <v>20</v>
       </c>
-      <c r="M20" s="9">
+      <c r="M20" s="8">
         <v>13.5</v>
       </c>
-      <c r="N20" s="9">
+      <c r="N20" s="8">
         <v>18</v>
       </c>
-      <c r="O20" s="9">
+      <c r="O20" s="8">
         <v>20</v>
       </c>
     </row>
@@ -1353,72 +1412,72 @@
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="12" t="s">
+      <c r="B21" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="7">
-        <v>0</v>
-      </c>
-      <c r="D21" s="7">
-        <v>0</v>
-      </c>
-      <c r="E21" s="7">
-        <v>0</v>
-      </c>
-      <c r="F21" s="7">
-        <v>0</v>
-      </c>
-      <c r="G21" s="7">
-        <v>0</v>
-      </c>
-      <c r="H21" s="7">
-        <v>0</v>
-      </c>
-      <c r="I21" s="7">
-        <v>0</v>
-      </c>
-      <c r="J21" s="7">
-        <v>0</v>
-      </c>
-      <c r="K21" s="7">
-        <v>0</v>
-      </c>
-      <c r="L21" s="7">
-        <v>0</v>
-      </c>
-      <c r="M21" s="7">
-        <v>0</v>
-      </c>
-      <c r="N21" s="7">
-        <v>0</v>
-      </c>
-      <c r="O21" s="7">
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0</v>
+      </c>
+      <c r="O21" s="6">
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="11" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="15"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15"/>
-      <c r="M23" s="15"/>
-      <c r="N23" s="15"/>
-      <c r="O23" s="15"/>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -1429,133 +1488,133 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="18" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="15" t="s">
+      <c r="A26" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="18" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <v>6.66</v>
       </c>
-      <c r="D27" s="9">
+      <c r="D27" s="8">
         <v>1.82</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <v>0.02</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="8">
         <v>0.17</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="8">
         <v>0.19</v>
       </c>
-      <c r="H27" s="9">
-        <v>0</v>
-      </c>
-      <c r="I27" s="9">
+      <c r="H27" s="8">
+        <v>0</v>
+      </c>
+      <c r="I27" s="8">
         <v>0.01</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="8">
         <v>0.01</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="8">
         <v>0.14000000000000001</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="8">
         <v>0.41</v>
       </c>
-      <c r="M27" s="9">
+      <c r="M27" s="8">
         <v>6.13</v>
       </c>
-      <c r="N27" s="9">
+      <c r="N27" s="8">
         <v>1.27</v>
       </c>
-      <c r="O27" s="9">
+      <c r="O27" s="8">
         <v>0.17</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.15">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <v>0.05</v>
       </c>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-      <c r="E28" s="9">
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+      <c r="E28" s="8">
         <v>0.01</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="8">
         <v>0.05</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="8">
         <v>0.06</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="8">
         <v>1.71</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="8">
         <v>8.65</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="8">
         <v>5.37</v>
       </c>
-      <c r="K28" s="9">
+      <c r="K28" s="8">
         <v>1.67</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="8">
         <v>0.81</v>
       </c>
-      <c r="M28" s="9">
+      <c r="M28" s="8">
         <v>0.36</v>
       </c>
-      <c r="N28" s="9">
+      <c r="N28" s="8">
         <v>0.45</v>
       </c>
-      <c r="O28" s="9">
+      <c r="O28" s="8">
         <v>0.55000000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="15"/>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -1629,238 +1688,2960 @@
       </c>
     </row>
     <row r="34" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
+      <c r="A34" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="16" t="s">
+      <c r="B34" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="17">
+      <c r="C34" s="14">
         <v>1161978</v>
       </c>
-      <c r="D34" s="17">
+      <c r="D34" s="14">
         <v>1179681</v>
       </c>
-      <c r="E34" s="17">
+      <c r="E34" s="14">
         <v>1197147</v>
       </c>
-      <c r="F34" s="17">
+      <c r="F34" s="14">
         <v>1214270</v>
       </c>
-      <c r="G34" s="17">
+      <c r="G34" s="14">
         <v>1230981</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H34" s="14">
         <v>1247236</v>
       </c>
-      <c r="I34" s="17">
+      <c r="I34" s="14">
         <v>1263066</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="14">
         <v>1278562</v>
       </c>
-      <c r="K34" s="17">
+      <c r="K34" s="14">
         <v>1293859</v>
       </c>
-      <c r="L34" s="17">
+      <c r="L34" s="14">
         <v>1309054</v>
       </c>
-      <c r="M34" s="17">
+      <c r="M34" s="14">
         <v>1324171</v>
       </c>
-      <c r="N34" s="17">
+      <c r="N34" s="14">
         <v>1339180</v>
       </c>
-      <c r="O34" s="17">
+      <c r="O34" s="14">
         <v>1354052</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="16" x14ac:dyDescent="0.15">
-      <c r="A35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="B35" s="16" t="s">
+      <c r="B35" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="8">
         <v>58.7</v>
       </c>
-      <c r="D35" s="9">
+      <c r="D35" s="8">
         <v>58.5</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="8">
         <v>58.5</v>
       </c>
-      <c r="F35" s="9">
+      <c r="F35" s="8">
         <v>58.5</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="8">
         <v>58.6</v>
       </c>
-      <c r="H35" s="9">
+      <c r="H35" s="8">
         <v>58.5</v>
       </c>
-      <c r="I35" s="9">
+      <c r="I35" s="8">
         <v>59</v>
       </c>
-      <c r="J35" s="9">
+      <c r="J35" s="8">
         <v>59.1</v>
       </c>
-      <c r="K35" s="9">
+      <c r="K35" s="8">
         <v>59.4</v>
       </c>
-      <c r="L35" s="9">
+      <c r="L35" s="8">
         <v>59.7</v>
       </c>
-      <c r="M35" s="9">
+      <c r="M35" s="8">
         <v>59.8</v>
       </c>
-      <c r="N35" s="9">
+      <c r="N35" s="8">
         <v>59.8</v>
       </c>
-      <c r="O35" s="9">
+      <c r="O35" s="8">
         <v>59.8</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
+      <c r="A36" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B36" s="16" t="s">
+      <c r="B36" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="D36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="G36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="H36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="K36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="L36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="M36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="N36" s="17" t="s">
-        <v>8</v>
-      </c>
-      <c r="O36" s="17" t="s">
+      <c r="C36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O36" s="14" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="16" x14ac:dyDescent="0.15">
-      <c r="A37" s="8" t="s">
+      <c r="A37" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="16" t="s">
+      <c r="B37" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C37" s="9">
+      <c r="C37" s="8">
         <v>26.48</v>
       </c>
-      <c r="D37" s="9">
+      <c r="D37" s="8">
         <v>27.99</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="8">
         <v>28.04</v>
       </c>
-      <c r="F37" s="9">
+      <c r="F37" s="8">
         <v>27.75</v>
       </c>
-      <c r="G37" s="9">
+      <c r="G37" s="8">
         <v>28.46</v>
       </c>
-      <c r="H37" s="9">
+      <c r="H37" s="8">
         <v>29.07</v>
       </c>
-      <c r="I37" s="9">
+      <c r="I37" s="8">
         <v>29.86</v>
       </c>
-      <c r="J37" s="9">
+      <c r="J37" s="8">
         <v>29.65</v>
       </c>
-      <c r="K37" s="9">
+      <c r="K37" s="8">
         <v>30.47</v>
       </c>
-      <c r="L37" s="9">
+      <c r="L37" s="8">
         <v>31.47</v>
       </c>
-      <c r="M37" s="9">
+      <c r="M37" s="8">
         <v>30.23</v>
       </c>
-      <c r="N37" s="9">
+      <c r="N37" s="8">
         <v>31.79</v>
       </c>
-      <c r="O37" s="9">
+      <c r="O37" s="8">
         <v>30.43</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="16" x14ac:dyDescent="0.15">
-      <c r="A38" s="8" t="s">
+      <c r="A38" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="B38" s="16" t="s">
+      <c r="B38" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C38" s="8">
         <v>2.62</v>
       </c>
-      <c r="D38" s="9">
+      <c r="D38" s="8">
         <v>2.71</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="8">
         <v>2.8</v>
       </c>
-      <c r="F38" s="9">
+      <c r="F38" s="8">
         <v>2.91</v>
       </c>
-      <c r="G38" s="9">
+      <c r="G38" s="8">
         <v>2.84</v>
       </c>
-      <c r="H38" s="9">
+      <c r="H38" s="8">
         <v>2.99</v>
       </c>
-      <c r="I38" s="9">
+      <c r="I38" s="8">
         <v>3.18</v>
       </c>
-      <c r="J38" s="9">
+      <c r="J38" s="8">
         <v>3.15</v>
       </c>
-      <c r="K38" s="9">
+      <c r="K38" s="8">
         <v>3.15</v>
       </c>
-      <c r="L38" s="9">
+      <c r="L38" s="8">
         <v>2.75</v>
       </c>
-      <c r="M38" s="9">
+      <c r="M38" s="8">
         <v>3.05</v>
       </c>
-      <c r="N38" s="9">
+      <c r="N38" s="8">
         <v>3.1</v>
       </c>
-      <c r="O38" s="9">
+      <c r="O38" s="8">
         <v>3.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A29:O29"/>
+    <mergeCell ref="B10:B21"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEE078D-9750-1D4E-BA37-4A7256F92070}">
+  <dimension ref="D4:R41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+    </row>
+    <row r="5" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="12"/>
+    </row>
+    <row r="6" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="H6" s="12"/>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="12"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="12"/>
+    </row>
+    <row r="7" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="12"/>
+      <c r="N7" s="12"/>
+      <c r="O7" s="12"/>
+      <c r="P7" s="12"/>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="12"/>
+    </row>
+    <row r="8" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
+      <c r="I8" s="12"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="12"/>
+      <c r="L8" s="12"/>
+      <c r="M8" s="12"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
+      <c r="P8" s="12"/>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="12"/>
+    </row>
+    <row r="9" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="12"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="12"/>
+      <c r="I9" s="12"/>
+      <c r="J9" s="12"/>
+      <c r="K9" s="12"/>
+      <c r="L9" s="12"/>
+      <c r="M9" s="12"/>
+      <c r="N9" s="12"/>
+      <c r="O9" s="12"/>
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12"/>
+      <c r="R9" s="12"/>
+    </row>
+    <row r="10" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
+      <c r="K10" s="12"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="12"/>
+      <c r="O10" s="12"/>
+      <c r="P10" s="12"/>
+      <c r="Q10" s="12"/>
+      <c r="R10" s="12"/>
+    </row>
+    <row r="11" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="12"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="12"/>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12"/>
+    </row>
+    <row r="12" spans="4:18" ht="28" x14ac:dyDescent="0.2">
+      <c r="D12" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="8">
+        <v>8.6</v>
+      </c>
+      <c r="G14" s="8">
+        <v>10</v>
+      </c>
+      <c r="H14" s="8">
+        <v>12</v>
+      </c>
+      <c r="I14" s="8">
+        <v>13.43</v>
+      </c>
+      <c r="J14" s="8">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="K14" s="8">
+        <v>17</v>
+      </c>
+      <c r="L14" s="8">
+        <v>21</v>
+      </c>
+      <c r="M14" s="8">
+        <v>24.5</v>
+      </c>
+      <c r="N14" s="8">
+        <v>21</v>
+      </c>
+      <c r="O14" s="8">
+        <v>23</v>
+      </c>
+      <c r="P14" s="8">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>13.5</v>
+      </c>
+      <c r="R14" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="8">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="G15" s="8">
+        <v>75.81</v>
+      </c>
+      <c r="H15" s="8">
+        <v>78.569999999999993</v>
+      </c>
+      <c r="I15" s="8">
+        <v>80.680000000000007</v>
+      </c>
+      <c r="J15" s="8">
+        <v>80.8</v>
+      </c>
+      <c r="K15" s="8">
+        <v>86.87</v>
+      </c>
+      <c r="L15" s="8">
+        <v>94.88</v>
+      </c>
+      <c r="M15" s="8">
+        <v>93.51</v>
+      </c>
+      <c r="N15" s="8">
+        <v>95.85</v>
+      </c>
+      <c r="O15" s="8">
+        <v>86.53</v>
+      </c>
+      <c r="P15" s="8">
+        <v>92.29</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>98.51</v>
+      </c>
+      <c r="R15" s="8">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="16" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="8">
+        <v>6.11</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1.82</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="N16" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="P16" s="8">
+        <v>5.75</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>1.65</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="8">
+        <v>74.02</v>
+      </c>
+      <c r="G18" s="8">
+        <v>75.62</v>
+      </c>
+      <c r="H18" s="8">
+        <v>77.16</v>
+      </c>
+      <c r="I18" s="8">
+        <v>78.13</v>
+      </c>
+      <c r="J18" s="8">
+        <v>80.03</v>
+      </c>
+      <c r="K18" s="8">
+        <v>82</v>
+      </c>
+      <c r="L18" s="8">
+        <v>84.59</v>
+      </c>
+      <c r="M18" s="8">
+        <v>91</v>
+      </c>
+      <c r="N18" s="8">
+        <v>90.5</v>
+      </c>
+      <c r="O18" s="8">
+        <v>89</v>
+      </c>
+      <c r="P18" s="8">
+        <v>104.1</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>95.15</v>
+      </c>
+      <c r="R18" s="8">
+        <v>97.25</v>
+      </c>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="10">
+        <v>68.17</v>
+      </c>
+      <c r="G19" s="10">
+        <v>69.02</v>
+      </c>
+      <c r="H19" s="10">
+        <v>70</v>
+      </c>
+      <c r="I19" s="10">
+        <v>71</v>
+      </c>
+      <c r="J19" s="10">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="K19" s="10">
+        <v>73</v>
+      </c>
+      <c r="L19" s="10">
+        <v>74.5</v>
+      </c>
+      <c r="M19" s="10">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="N19" s="10">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="O19" s="10">
+        <v>78.2</v>
+      </c>
+      <c r="P19" s="10">
+        <v>79.2</v>
+      </c>
+      <c r="Q19" s="10">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="R19" s="10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1.43</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1.48</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1.52</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="J20" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="K20" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="L20" s="10">
+        <v>3</v>
+      </c>
+      <c r="M20" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="N20" s="10">
+        <v>5</v>
+      </c>
+      <c r="O20" s="10">
+        <v>5</v>
+      </c>
+      <c r="P20" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>5</v>
+      </c>
+      <c r="R20" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="10">
+        <v>4.42</v>
+      </c>
+      <c r="G21" s="10">
+        <v>5.12</v>
+      </c>
+      <c r="H21" s="10">
+        <v>5.64</v>
+      </c>
+      <c r="I21" s="10">
+        <v>5.53</v>
+      </c>
+      <c r="J21" s="10">
+        <v>5.43</v>
+      </c>
+      <c r="K21" s="10">
+        <v>6.5</v>
+      </c>
+      <c r="L21" s="10">
+        <v>7.09</v>
+      </c>
+      <c r="M21" s="10">
+        <v>10.9</v>
+      </c>
+      <c r="N21" s="10">
+        <v>8.6</v>
+      </c>
+      <c r="O21" s="10">
+        <v>5.8</v>
+      </c>
+      <c r="P21" s="10">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="R21" s="10">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="L22" s="8">
+        <v>6.8</v>
+      </c>
+      <c r="M22" s="8">
+        <v>6.03</v>
+      </c>
+      <c r="N22" s="8">
+        <v>3.38</v>
+      </c>
+      <c r="O22" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="P22" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>0.51</v>
+      </c>
+      <c r="R22" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="8">
+        <v>10</v>
+      </c>
+      <c r="G23" s="8">
+        <v>12</v>
+      </c>
+      <c r="H23" s="8">
+        <v>13.43</v>
+      </c>
+      <c r="I23" s="8">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="J23" s="8">
+        <v>17</v>
+      </c>
+      <c r="K23" s="8">
+        <v>21</v>
+      </c>
+      <c r="L23" s="8">
+        <v>24.5</v>
+      </c>
+      <c r="M23" s="8">
+        <v>21</v>
+      </c>
+      <c r="N23" s="8">
+        <v>23</v>
+      </c>
+      <c r="O23" s="8">
+        <v>20</v>
+      </c>
+      <c r="P23" s="8">
+        <v>13.5</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>18</v>
+      </c>
+      <c r="R23" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6">
+        <v>0</v>
+      </c>
+      <c r="L24" s="6">
+        <v>0</v>
+      </c>
+      <c r="M24" s="6">
+        <v>0</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>0</v>
+      </c>
+      <c r="R24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D25" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+    </row>
+    <row r="26" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D26" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+    </row>
+    <row r="27" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="12"/>
+      <c r="N27" s="12"/>
+      <c r="O27" s="12"/>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+    </row>
+    <row r="28" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D28" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+    </row>
+    <row r="29" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D29" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="12"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="12"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12"/>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="12"/>
+    </row>
+    <row r="30" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D30" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="8">
+        <v>6.66</v>
+      </c>
+      <c r="G30" s="8">
+        <v>1.82</v>
+      </c>
+      <c r="H30" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="J30" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="K30" s="8">
+        <v>0</v>
+      </c>
+      <c r="L30" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="M30" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="N30" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O30" s="8">
+        <v>0.41</v>
+      </c>
+      <c r="P30" s="8">
+        <v>6.13</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>1.27</v>
+      </c>
+      <c r="R30" s="8">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="31" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D31" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0</v>
+      </c>
+      <c r="H31" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="I31" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1.71</v>
+      </c>
+      <c r="L31" s="8">
+        <v>8.65</v>
+      </c>
+      <c r="M31" s="8">
+        <v>5.37</v>
+      </c>
+      <c r="N31" s="8">
+        <v>1.67</v>
+      </c>
+      <c r="O31" s="8">
+        <v>0.81</v>
+      </c>
+      <c r="P31" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="R31" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D32" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
+      <c r="H32" s="18"/>
+      <c r="I32" s="18"/>
+      <c r="J32" s="18"/>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="18"/>
+      <c r="O32" s="18"/>
+      <c r="P32" s="18"/>
+      <c r="Q32" s="18"/>
+      <c r="R32" s="18"/>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="12"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="12"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="12"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12"/>
+      <c r="Q33" s="12"/>
+      <c r="R33" s="12"/>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D34" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="12"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="12"/>
+      <c r="I34" s="12"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="M34" s="12"/>
+      <c r="N34" s="12"/>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12"/>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="12"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="12"/>
+      <c r="J35" s="12"/>
+      <c r="K35" s="12"/>
+      <c r="L35" s="12"/>
+      <c r="M35" s="12"/>
+      <c r="N35" s="12"/>
+      <c r="O35" s="12"/>
+      <c r="P35" s="12"/>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="12"/>
+    </row>
+    <row r="36" spans="4:18" ht="28" x14ac:dyDescent="0.2">
+      <c r="D36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D37" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="14">
+        <v>1161978</v>
+      </c>
+      <c r="G37" s="14">
+        <v>1179681</v>
+      </c>
+      <c r="H37" s="14">
+        <v>1197147</v>
+      </c>
+      <c r="I37" s="14">
+        <v>1214270</v>
+      </c>
+      <c r="J37" s="14">
+        <v>1230981</v>
+      </c>
+      <c r="K37" s="14">
+        <v>1247236</v>
+      </c>
+      <c r="L37" s="14">
+        <v>1263066</v>
+      </c>
+      <c r="M37" s="14">
+        <v>1278562</v>
+      </c>
+      <c r="N37" s="14">
+        <v>1293859</v>
+      </c>
+      <c r="O37" s="14">
+        <v>1309054</v>
+      </c>
+      <c r="P37" s="14">
+        <v>1324171</v>
+      </c>
+      <c r="Q37" s="14">
+        <v>1339180</v>
+      </c>
+      <c r="R37" s="14">
+        <v>1354052</v>
+      </c>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D38" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F38" s="8">
+        <v>58.7</v>
+      </c>
+      <c r="G38" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="H38" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="I38" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="J38" s="8">
+        <v>58.6</v>
+      </c>
+      <c r="K38" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="L38" s="8">
+        <v>59</v>
+      </c>
+      <c r="M38" s="8">
+        <v>59.1</v>
+      </c>
+      <c r="N38" s="8">
+        <v>59.4</v>
+      </c>
+      <c r="O38" s="8">
+        <v>59.7</v>
+      </c>
+      <c r="P38" s="8">
+        <v>59.8</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>59.8</v>
+      </c>
+      <c r="R38" s="8">
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D39" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R39" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D40" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="8">
+        <v>26.48</v>
+      </c>
+      <c r="G40" s="8">
+        <v>27.99</v>
+      </c>
+      <c r="H40" s="8">
+        <v>28.04</v>
+      </c>
+      <c r="I40" s="8">
+        <v>27.75</v>
+      </c>
+      <c r="J40" s="8">
+        <v>28.46</v>
+      </c>
+      <c r="K40" s="8">
+        <v>29.07</v>
+      </c>
+      <c r="L40" s="8">
+        <v>29.86</v>
+      </c>
+      <c r="M40" s="8">
+        <v>29.65</v>
+      </c>
+      <c r="N40" s="8">
+        <v>30.47</v>
+      </c>
+      <c r="O40" s="8">
+        <v>31.47</v>
+      </c>
+      <c r="P40" s="8">
+        <v>30.23</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>31.79</v>
+      </c>
+      <c r="R40" s="8">
+        <v>30.43</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D41" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F41" s="8">
+        <v>2.62</v>
+      </c>
+      <c r="G41" s="8">
+        <v>2.71</v>
+      </c>
+      <c r="H41" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="I41" s="8">
+        <v>2.91</v>
+      </c>
+      <c r="J41" s="8">
+        <v>2.84</v>
+      </c>
+      <c r="K41" s="8">
+        <v>2.99</v>
+      </c>
+      <c r="L41" s="8">
+        <v>3.18</v>
+      </c>
+      <c r="M41" s="8">
+        <v>3.15</v>
+      </c>
+      <c r="N41" s="8">
+        <v>3.15</v>
+      </c>
+      <c r="O41" s="8">
+        <v>2.75</v>
+      </c>
+      <c r="P41" s="8">
+        <v>3.05</v>
+      </c>
+      <c r="Q41" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="R41" s="8">
+        <v>3.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="D32:R32"/>
+    <mergeCell ref="E13:E24"/>
+    <mergeCell ref="D26:R26"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29247090-4910-F043-A63D-FDDD8732C11E}">
+  <dimension ref="A1:O38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="16"/>
+      <c r="N3" s="16"/>
+      <c r="O3" s="16"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16"/>
+      <c r="O4" s="16"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="16"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+    </row>
+    <row r="9" spans="1:15" ht="28" x14ac:dyDescent="0.2">
+      <c r="A9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="8">
+        <v>15.55</v>
+      </c>
+      <c r="D11" s="8">
+        <v>12.41</v>
+      </c>
+      <c r="E11" s="8">
+        <v>8.32</v>
+      </c>
+      <c r="F11" s="8">
+        <v>17.87</v>
+      </c>
+      <c r="G11" s="8">
+        <v>26.55</v>
+      </c>
+      <c r="H11" s="8">
+        <v>23.49</v>
+      </c>
+      <c r="I11" s="8">
+        <v>20.21</v>
+      </c>
+      <c r="J11" s="8">
+        <v>19.54</v>
+      </c>
+      <c r="K11" s="8">
+        <v>16.07</v>
+      </c>
+      <c r="L11" s="8">
+        <v>20.48</v>
+      </c>
+      <c r="M11" s="8">
+        <v>26.55</v>
+      </c>
+      <c r="N11" s="8">
+        <v>32.130000000000003</v>
+      </c>
+      <c r="O11" s="8">
+        <v>29.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8">
+        <v>49.22</v>
+      </c>
+      <c r="D12" s="8">
+        <v>55.82</v>
+      </c>
+      <c r="E12" s="8">
+        <v>68.36</v>
+      </c>
+      <c r="F12" s="8">
+        <v>60.12</v>
+      </c>
+      <c r="G12" s="8">
+        <v>58.87</v>
+      </c>
+      <c r="H12" s="8">
+        <v>54.24</v>
+      </c>
+      <c r="I12" s="8">
+        <v>61.3</v>
+      </c>
+      <c r="J12" s="8">
+        <v>58.11</v>
+      </c>
+      <c r="K12" s="8">
+        <v>55.15</v>
+      </c>
+      <c r="L12" s="8">
+        <v>56.12</v>
+      </c>
+      <c r="M12" s="8">
+        <v>62.83</v>
+      </c>
+      <c r="N12" s="8">
+        <v>47.38</v>
+      </c>
+      <c r="O12" s="8">
+        <v>51.29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8">
+        <v>3.32</v>
+      </c>
+      <c r="D13" s="8">
+        <v>3.07</v>
+      </c>
+      <c r="E13" s="8">
+        <v>3.46</v>
+      </c>
+      <c r="F13" s="8">
+        <v>3.23</v>
+      </c>
+      <c r="G13" s="8">
+        <v>2.64</v>
+      </c>
+      <c r="H13" s="8">
+        <v>3.08</v>
+      </c>
+      <c r="I13" s="8">
+        <v>3.38</v>
+      </c>
+      <c r="J13" s="8">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="K13" s="8">
+        <v>4.12</v>
+      </c>
+      <c r="L13" s="8">
+        <v>3.07</v>
+      </c>
+      <c r="M13" s="8">
+        <v>3.21</v>
+      </c>
+      <c r="N13" s="8">
+        <v>4.28</v>
+      </c>
+      <c r="O13" s="8">
+        <v>3.95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="8">
+        <v>30.94</v>
+      </c>
+      <c r="D15" s="8">
+        <v>28.61</v>
+      </c>
+      <c r="E15" s="8">
+        <v>34.64</v>
+      </c>
+      <c r="F15" s="8">
+        <v>30.73</v>
+      </c>
+      <c r="G15" s="8">
+        <v>29.42</v>
+      </c>
+      <c r="H15" s="8">
+        <v>31.99</v>
+      </c>
+      <c r="I15" s="8">
+        <v>37.81</v>
+      </c>
+      <c r="J15" s="8">
+        <v>34.26</v>
+      </c>
+      <c r="K15" s="8">
+        <v>31.33</v>
+      </c>
+      <c r="L15" s="8">
+        <v>31.94</v>
+      </c>
+      <c r="M15" s="8">
+        <v>31.86</v>
+      </c>
+      <c r="N15" s="8">
+        <v>29.36</v>
+      </c>
+      <c r="O15" s="8">
+        <v>30.16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10">
+        <v>25.53</v>
+      </c>
+      <c r="D16" s="10">
+        <v>25.8</v>
+      </c>
+      <c r="E16" s="10">
+        <v>25.22</v>
+      </c>
+      <c r="F16" s="10">
+        <v>24.97</v>
+      </c>
+      <c r="G16" s="10">
+        <v>25.31</v>
+      </c>
+      <c r="H16" s="10">
+        <v>25.58</v>
+      </c>
+      <c r="I16" s="10">
+        <v>25.75</v>
+      </c>
+      <c r="J16" s="10">
+        <v>26</v>
+      </c>
+      <c r="K16" s="10">
+        <v>26.3</v>
+      </c>
+      <c r="L16" s="10">
+        <v>26.5</v>
+      </c>
+      <c r="M16" s="10">
+        <v>26.7</v>
+      </c>
+      <c r="N16" s="10">
+        <v>26.9</v>
+      </c>
+      <c r="O16" s="10">
+        <v>27.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="10">
+        <v>3.19</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.43</v>
+      </c>
+      <c r="E17" s="10">
+        <v>7.3</v>
+      </c>
+      <c r="F17" s="10">
+        <v>3.87</v>
+      </c>
+      <c r="G17" s="10">
+        <v>2.31</v>
+      </c>
+      <c r="H17" s="10">
+        <v>4.32</v>
+      </c>
+      <c r="I17" s="10">
+        <v>9.94</v>
+      </c>
+      <c r="J17" s="10">
+        <v>6.21</v>
+      </c>
+      <c r="K17" s="10">
+        <v>3.09</v>
+      </c>
+      <c r="L17" s="10">
+        <v>4.07</v>
+      </c>
+      <c r="M17" s="10">
+        <v>4.37</v>
+      </c>
+      <c r="N17" s="10">
+        <v>1.39</v>
+      </c>
+      <c r="O17" s="10">
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2.23</v>
+      </c>
+      <c r="D18" s="10">
+        <v>2.38</v>
+      </c>
+      <c r="E18" s="10">
+        <v>2.12</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1.89</v>
+      </c>
+      <c r="G18" s="10">
+        <v>1.8</v>
+      </c>
+      <c r="H18" s="10">
+        <v>2.1</v>
+      </c>
+      <c r="I18" s="10">
+        <v>2.12</v>
+      </c>
+      <c r="J18" s="10">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="K18" s="10">
+        <v>1.94</v>
+      </c>
+      <c r="L18" s="10">
+        <v>1.38</v>
+      </c>
+      <c r="M18" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="N18" s="10">
+        <v>1.07</v>
+      </c>
+      <c r="O18" s="10">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="8">
+        <v>24.73</v>
+      </c>
+      <c r="D19" s="8">
+        <v>34.36</v>
+      </c>
+      <c r="E19" s="8">
+        <v>27.64</v>
+      </c>
+      <c r="F19" s="8">
+        <v>23.93</v>
+      </c>
+      <c r="G19" s="8">
+        <v>35.15</v>
+      </c>
+      <c r="H19" s="8">
+        <v>28.61</v>
+      </c>
+      <c r="I19" s="8">
+        <v>27.54</v>
+      </c>
+      <c r="J19" s="8">
+        <v>32.01</v>
+      </c>
+      <c r="K19" s="8">
+        <v>23.52</v>
+      </c>
+      <c r="L19" s="8">
+        <v>21.17</v>
+      </c>
+      <c r="M19" s="8">
+        <v>28.6</v>
+      </c>
+      <c r="N19" s="8">
+        <v>24.52</v>
+      </c>
+      <c r="O19" s="8">
+        <v>26.26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="8">
+        <v>12.41</v>
+      </c>
+      <c r="D20" s="8">
+        <v>8.32</v>
+      </c>
+      <c r="E20" s="8">
+        <v>17.87</v>
+      </c>
+      <c r="F20" s="8">
+        <v>26.55</v>
+      </c>
+      <c r="G20" s="8">
+        <v>23.49</v>
+      </c>
+      <c r="H20" s="8">
+        <v>20.21</v>
+      </c>
+      <c r="I20" s="8">
+        <v>19.54</v>
+      </c>
+      <c r="J20" s="8">
+        <v>16.07</v>
+      </c>
+      <c r="K20" s="8">
+        <v>20.48</v>
+      </c>
+      <c r="L20" s="8">
+        <v>26.55</v>
+      </c>
+      <c r="M20" s="8">
+        <v>32.130000000000003</v>
+      </c>
+      <c r="N20" s="8">
+        <v>29.91</v>
+      </c>
+      <c r="O20" s="8">
+        <v>28.72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0</v>
+      </c>
+      <c r="O21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="16"/>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16"/>
+      <c r="O22" s="16"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="18"/>
+      <c r="D23" s="18"/>
+      <c r="E23" s="18"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18"/>
+      <c r="I23" s="18"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="16"/>
+      <c r="O24" s="16"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="16"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="16"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="16"/>
+      <c r="O25" s="16"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="16"/>
+      <c r="O26" s="16"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="8">
+        <v>2.88</v>
+      </c>
+      <c r="D27" s="8">
+        <v>2.5</v>
+      </c>
+      <c r="E27" s="8">
+        <v>2.99</v>
+      </c>
+      <c r="F27" s="8">
+        <v>2.74</v>
+      </c>
+      <c r="G27" s="8">
+        <v>2.09</v>
+      </c>
+      <c r="H27" s="8">
+        <v>2.4900000000000002</v>
+      </c>
+      <c r="I27" s="8">
+        <v>2.93</v>
+      </c>
+      <c r="J27" s="8">
+        <v>4.1900000000000004</v>
+      </c>
+      <c r="K27" s="8">
+        <v>3.37</v>
+      </c>
+      <c r="L27" s="8">
+        <v>2.4500000000000002</v>
+      </c>
+      <c r="M27" s="8">
+        <v>3.29</v>
+      </c>
+      <c r="N27" s="8">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="O27" s="8">
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="8">
+        <v>24.65</v>
+      </c>
+      <c r="D28" s="8">
+        <v>34.07</v>
+      </c>
+      <c r="E28" s="8">
+        <v>26.92</v>
+      </c>
+      <c r="F28" s="8">
+        <v>23.99</v>
+      </c>
+      <c r="G28" s="8">
+        <v>35.83</v>
+      </c>
+      <c r="H28" s="8">
+        <v>27.92</v>
+      </c>
+      <c r="I28" s="8">
+        <v>27.6</v>
+      </c>
+      <c r="J28" s="8">
+        <v>31.63</v>
+      </c>
+      <c r="K28" s="8">
+        <v>22.82</v>
+      </c>
+      <c r="L28" s="8">
+        <v>21.59</v>
+      </c>
+      <c r="M28" s="8">
+        <v>29.32</v>
+      </c>
+      <c r="N28" s="8">
+        <v>23.07</v>
+      </c>
+      <c r="O28" s="8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="16"/>
+      <c r="D30" s="16"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16"/>
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="16"/>
+      <c r="K30" s="16"/>
+      <c r="L30" s="16"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="16"/>
+      <c r="O30" s="16"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="16"/>
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="16"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="16"/>
+      <c r="K31" s="16"/>
+      <c r="L31" s="16"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="16"/>
+      <c r="O31" s="16"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="16"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="16"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="16"/>
+      <c r="K32" s="16"/>
+      <c r="L32" s="16"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="16"/>
+      <c r="O32" s="16"/>
+    </row>
+    <row r="33" spans="1:15" ht="28" x14ac:dyDescent="0.2">
+      <c r="A33" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="14">
+        <v>297827</v>
+      </c>
+      <c r="D34" s="14">
+        <v>300595</v>
+      </c>
+      <c r="E34" s="14">
+        <v>303374</v>
+      </c>
+      <c r="F34" s="14">
+        <v>306076</v>
+      </c>
+      <c r="G34" s="14">
+        <v>308641</v>
+      </c>
+      <c r="H34" s="14">
+        <v>311051</v>
+      </c>
+      <c r="I34" s="14">
+        <v>313335</v>
+      </c>
+      <c r="J34" s="14">
+        <v>315537</v>
+      </c>
+      <c r="K34" s="14">
+        <v>317719</v>
+      </c>
+      <c r="L34" s="14">
+        <v>319929</v>
+      </c>
+      <c r="M34" s="14">
+        <v>322180</v>
+      </c>
+      <c r="N34" s="14">
+        <v>324459</v>
+      </c>
+      <c r="O34" s="14">
+        <v>326767</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="8">
+        <v>85.7</v>
+      </c>
+      <c r="D35" s="8">
+        <v>85.8</v>
+      </c>
+      <c r="E35" s="8">
+        <v>83.1</v>
+      </c>
+      <c r="F35" s="8">
+        <v>81.599999999999994</v>
+      </c>
+      <c r="G35" s="8">
+        <v>82</v>
+      </c>
+      <c r="H35" s="8">
+        <v>82.2</v>
+      </c>
+      <c r="I35" s="8">
+        <v>82.2</v>
+      </c>
+      <c r="J35" s="8">
+        <v>82.4</v>
+      </c>
+      <c r="K35" s="8">
+        <v>82.8</v>
+      </c>
+      <c r="L35" s="8">
+        <v>82.8</v>
+      </c>
+      <c r="M35" s="8">
+        <v>82.9</v>
+      </c>
+      <c r="N35" s="8">
+        <v>82.9</v>
+      </c>
+      <c r="O35" s="8">
+        <v>82.9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O36" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="8">
+        <v>18.940000000000001</v>
+      </c>
+      <c r="D37" s="8">
+        <v>20.64</v>
+      </c>
+      <c r="E37" s="8">
+        <v>22.54</v>
+      </c>
+      <c r="F37" s="8">
+        <v>20.190000000000001</v>
+      </c>
+      <c r="G37" s="8">
+        <v>19.27</v>
+      </c>
+      <c r="H37" s="8">
+        <v>18.489999999999998</v>
+      </c>
+      <c r="I37" s="8">
+        <v>19.73</v>
+      </c>
+      <c r="J37" s="8">
+        <v>18.350000000000001</v>
+      </c>
+      <c r="K37" s="8">
+        <v>18.77</v>
+      </c>
+      <c r="L37" s="8">
+        <v>19.149999999999999</v>
+      </c>
+      <c r="M37" s="8">
+        <v>17.75</v>
+      </c>
+      <c r="N37" s="8">
+        <v>15.19</v>
+      </c>
+      <c r="O37" s="8">
+        <v>16.03</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="8">
+        <v>2.6</v>
+      </c>
+      <c r="D38" s="8">
+        <v>2.71</v>
+      </c>
+      <c r="E38" s="8">
+        <v>3.03</v>
+      </c>
+      <c r="F38" s="8">
+        <v>2.98</v>
+      </c>
+      <c r="G38" s="8">
+        <v>3.06</v>
+      </c>
+      <c r="H38" s="8">
+        <v>2.93</v>
+      </c>
+      <c r="I38" s="8">
+        <v>3.11</v>
+      </c>
+      <c r="J38" s="8">
+        <v>3.17</v>
+      </c>
+      <c r="K38" s="8">
+        <v>2.94</v>
+      </c>
+      <c r="L38" s="8">
+        <v>2.93</v>
+      </c>
+      <c r="M38" s="8">
+        <v>3.54</v>
+      </c>
+      <c r="N38" s="8">
+        <v>3.12</v>
+      </c>
+      <c r="O38" s="8">
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Abhinav | Notebook for table similarities
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/informationist/Projects/src/github.com/usc-isi-i2/sheet_annotator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF2A525-575A-B94E-9738-AD72E9FC34B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DAE892-819F-BF45-B9B5-C1CC9288D21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="2" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
+    <workbookView xWindow="-38400" yWindow="-4440" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
   </bookViews>
   <sheets>
     <sheet name="india_wheat" sheetId="1" r:id="rId1"/>
@@ -770,12 +770,12 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="39.5" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="44.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="8.83203125" style="3"/>
   </cols>
@@ -1939,7 +1939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEE078D-9750-1D4E-BA37-4A7256F92070}">
   <dimension ref="D4:R41"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E13" sqref="E13:E24"/>
     </sheetView>
   </sheetViews>
@@ -3300,11 +3300,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29247090-4910-F043-A63D-FDDD8732C11E}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
Abhinav | Use similar blocks between source and target for bounds
* Use target sheet start and ends as default bounds
* For similar tables use the table bounds
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/informationist/Projects/src/github.com/usc-isi-i2/sheet_annotator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99DAE892-819F-BF45-B9B5-C1CC9288D21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0B3EF9-EBB9-EA41-9989-067A6DF01BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4440" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
+    <workbookView xWindow="-38400" yWindow="-4440" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
   </bookViews>
   <sheets>
     <sheet name="india_wheat" sheetId="1" r:id="rId1"/>
     <sheet name="shifted_india_wheat" sheetId="3" r:id="rId2"/>
-    <sheet name="usa_wheat" sheetId="4" r:id="rId3"/>
+    <sheet name="shifted_india_wheat_wo_anchors" sheetId="6" r:id="rId3"/>
+    <sheet name="usa_wheat" sheetId="4" r:id="rId4"/>
+    <sheet name="argentina_wheat" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="100">
   <si>
     <t>Data Last Updated on:</t>
   </si>
@@ -288,6 +290,54 @@
   </si>
   <si>
     <t>For example, in the 2017/18 balance, the NMY refers to the crop that is harvested from June 2017 to September 2017 and marketed between June 2017 and May 2018</t>
+  </si>
+  <si>
+    <t>ARGENTINA</t>
+  </si>
+  <si>
+    <t>December/November</t>
+  </si>
+  <si>
+    <t>18.10</t>
+  </si>
+  <si>
+    <t>19.94</t>
+  </si>
+  <si>
+    <t>12.76</t>
+  </si>
+  <si>
+    <t>10.42</t>
+  </si>
+  <si>
+    <t>17.14</t>
+  </si>
+  <si>
+    <t>17.99</t>
+  </si>
+  <si>
+    <t>9.19</t>
+  </si>
+  <si>
+    <t>9.95</t>
+  </si>
+  <si>
+    <t>16.48</t>
+  </si>
+  <si>
+    <t>17.10</t>
+  </si>
+  <si>
+    <t>20.51</t>
+  </si>
+  <si>
+    <t>19.80</t>
+  </si>
+  <si>
+    <t>21.01</t>
+  </si>
+  <si>
+    <t>For example, in the 2017/18 balance, the NMY refers to the crop that is harvested from November 2017 to January 2018 and marketed between December 2017 and November 2018</t>
   </si>
 </sst>
 </file>
@@ -407,7 +457,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -441,6 +491,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -895,7 +960,7 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -942,7 +1007,7 @@
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="8">
@@ -989,7 +1054,7 @@
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="8">
@@ -1036,7 +1101,7 @@
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="8">
@@ -1083,7 +1148,7 @@
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1130,7 +1195,7 @@
       <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="8">
@@ -1177,7 +1242,7 @@
       <c r="A16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="10">
@@ -1224,7 +1289,7 @@
       <c r="A17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="10">
@@ -1271,7 +1336,7 @@
       <c r="A18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="10">
@@ -1318,7 +1383,7 @@
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="8">
@@ -1365,7 +1430,7 @@
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="8">
@@ -1412,7 +1477,7 @@
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="6">
@@ -1461,23 +1526,23 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -1488,18 +1553,18 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="23" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="18" t="s">
+      <c r="A26" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="23" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1507,7 +1572,7 @@
       <c r="A27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="8">
@@ -1554,7 +1619,7 @@
       <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="8">
@@ -1598,23 +1663,23 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -1939,8 +2004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEE078D-9750-1D4E-BA37-4A7256F92070}">
   <dimension ref="D4:R41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13:E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2164,7 +2229,7 @@
       <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -2211,7 +2276,7 @@
       <c r="D14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="19" t="s">
+      <c r="E14" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="8">
@@ -2258,7 +2323,7 @@
       <c r="D15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="8">
@@ -2305,7 +2370,7 @@
       <c r="D16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="19" t="s">
+      <c r="E16" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="8">
@@ -2352,7 +2417,7 @@
       <c r="D17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -2399,7 +2464,7 @@
       <c r="D18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="19" t="s">
+      <c r="E18" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="8">
@@ -2446,7 +2511,7 @@
       <c r="D19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="10">
@@ -2493,7 +2558,7 @@
       <c r="D20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="10">
@@ -2540,7 +2605,7 @@
       <c r="D21" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="19" t="s">
+      <c r="E21" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="10">
@@ -2587,7 +2652,7 @@
       <c r="D22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="19" t="s">
+      <c r="E22" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="8">
@@ -2634,7 +2699,7 @@
       <c r="D23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F23" s="8">
@@ -2681,7 +2746,7 @@
       <c r="D24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="6">
@@ -2744,23 +2809,23 @@
       <c r="R25" s="12"/>
     </row>
     <row r="26" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="22" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18"/>
-      <c r="R26" s="18"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23"/>
+      <c r="R26" s="23"/>
     </row>
     <row r="27" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D27" s="12" t="s">
@@ -2784,10 +2849,10 @@
       <c r="R27" s="12"/>
     </row>
     <row r="28" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="18" t="s">
+      <c r="E28" s="23" t="s">
         <v>54</v>
       </c>
       <c r="F28" s="12"/>
@@ -2805,10 +2870,10 @@
       <c r="R28" s="12"/>
     </row>
     <row r="29" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D29" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="18" t="s">
+      <c r="D29" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="23" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="12"/>
@@ -2829,7 +2894,7 @@
       <c r="D30" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="19" t="s">
+      <c r="E30" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F30" s="8">
@@ -2876,7 +2941,7 @@
       <c r="D31" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="19" t="s">
+      <c r="E31" s="24" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="8">
@@ -2920,23 +2985,23 @@
       </c>
     </row>
     <row r="32" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D32" s="17" t="s">
+      <c r="D32" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="18"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
-      <c r="H32" s="18"/>
-      <c r="I32" s="18"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="18"/>
-      <c r="L32" s="18"/>
-      <c r="M32" s="18"/>
-      <c r="N32" s="18"/>
-      <c r="O32" s="18"/>
-      <c r="P32" s="18"/>
-      <c r="Q32" s="18"/>
-      <c r="R32" s="18"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
     </row>
     <row r="33" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D33" s="12" t="s">
@@ -3297,16 +3362,1313 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B5EE06-08CE-BF4A-884D-58CF4ACB1707}">
+  <dimension ref="D4:R41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="G48" sqref="G48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D4" s="1"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="20"/>
+      <c r="J4" s="20"/>
+      <c r="K4" s="20"/>
+      <c r="L4" s="20"/>
+      <c r="M4" s="20"/>
+      <c r="N4" s="20"/>
+      <c r="O4" s="20"/>
+      <c r="P4" s="20"/>
+      <c r="Q4" s="20"/>
+      <c r="R4" s="20"/>
+    </row>
+    <row r="5" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="20"/>
+      <c r="N5" s="20"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+    </row>
+    <row r="6" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D6" s="1"/>
+      <c r="E6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+    </row>
+    <row r="7" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="20"/>
+      <c r="G7" s="20"/>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
+      <c r="N7" s="20"/>
+      <c r="O7" s="20"/>
+      <c r="P7" s="20"/>
+      <c r="Q7" s="20"/>
+      <c r="R7" s="20"/>
+    </row>
+    <row r="8" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+    </row>
+    <row r="9" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" s="20"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
+      <c r="I9" s="20"/>
+      <c r="J9" s="20"/>
+      <c r="K9" s="20"/>
+      <c r="L9" s="20"/>
+      <c r="M9" s="20"/>
+      <c r="N9" s="20"/>
+      <c r="O9" s="20"/>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+    </row>
+    <row r="10" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="20"/>
+      <c r="O10" s="20"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+    </row>
+    <row r="11" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="20"/>
+      <c r="G11" s="20"/>
+      <c r="H11" s="20"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="20"/>
+      <c r="K11" s="20"/>
+      <c r="L11" s="20"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20"/>
+      <c r="O11" s="20"/>
+      <c r="P11" s="20"/>
+      <c r="Q11" s="20"/>
+      <c r="R11" s="20"/>
+    </row>
+    <row r="12" spans="4:18" ht="28" x14ac:dyDescent="0.2">
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q12" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R12" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L13" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D14" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="8">
+        <v>8.6</v>
+      </c>
+      <c r="G14" s="8">
+        <v>10</v>
+      </c>
+      <c r="H14" s="8">
+        <v>12</v>
+      </c>
+      <c r="I14" s="8">
+        <v>13.43</v>
+      </c>
+      <c r="J14" s="8">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="K14" s="8">
+        <v>17</v>
+      </c>
+      <c r="L14" s="8">
+        <v>21</v>
+      </c>
+      <c r="M14" s="8">
+        <v>24.5</v>
+      </c>
+      <c r="N14" s="8">
+        <v>21</v>
+      </c>
+      <c r="O14" s="8">
+        <v>23</v>
+      </c>
+      <c r="P14" s="8">
+        <v>20</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>13.5</v>
+      </c>
+      <c r="R14" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D15" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="8">
+        <v>69.349999999999994</v>
+      </c>
+      <c r="G15" s="8">
+        <v>75.81</v>
+      </c>
+      <c r="H15" s="8">
+        <v>78.569999999999993</v>
+      </c>
+      <c r="I15" s="8">
+        <v>80.680000000000007</v>
+      </c>
+      <c r="J15" s="8">
+        <v>80.8</v>
+      </c>
+      <c r="K15" s="8">
+        <v>86.87</v>
+      </c>
+      <c r="L15" s="8">
+        <v>94.88</v>
+      </c>
+      <c r="M15" s="8">
+        <v>93.51</v>
+      </c>
+      <c r="N15" s="8">
+        <v>95.85</v>
+      </c>
+      <c r="O15" s="8">
+        <v>86.53</v>
+      </c>
+      <c r="P15" s="8">
+        <v>92.29</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>98.51</v>
+      </c>
+      <c r="R15" s="8">
+        <v>99.7</v>
+      </c>
+    </row>
+    <row r="16" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D16" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F16" s="8">
+        <v>6.11</v>
+      </c>
+      <c r="G16" s="8">
+        <v>1.82</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="I16" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="J16" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="K16" s="8">
+        <v>0</v>
+      </c>
+      <c r="L16" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="M16" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="N16" s="8">
+        <v>0.03</v>
+      </c>
+      <c r="O16" s="8">
+        <v>0.52</v>
+      </c>
+      <c r="P16" s="8">
+        <v>5.75</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>1.65</v>
+      </c>
+      <c r="R16" s="8">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="17" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="P17" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D18" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="8">
+        <v>74.02</v>
+      </c>
+      <c r="G18" s="8">
+        <v>75.62</v>
+      </c>
+      <c r="H18" s="8">
+        <v>77.16</v>
+      </c>
+      <c r="I18" s="8">
+        <v>78.13</v>
+      </c>
+      <c r="J18" s="8">
+        <v>80.03</v>
+      </c>
+      <c r="K18" s="8">
+        <v>82</v>
+      </c>
+      <c r="L18" s="8">
+        <v>84.59</v>
+      </c>
+      <c r="M18" s="8">
+        <v>91</v>
+      </c>
+      <c r="N18" s="8">
+        <v>90.5</v>
+      </c>
+      <c r="O18" s="8">
+        <v>89</v>
+      </c>
+      <c r="P18" s="8">
+        <v>104.1</v>
+      </c>
+      <c r="Q18" s="8">
+        <v>95.15</v>
+      </c>
+      <c r="R18" s="8">
+        <v>97.25</v>
+      </c>
+    </row>
+    <row r="19" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D19" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F19" s="10">
+        <v>68.17</v>
+      </c>
+      <c r="G19" s="10">
+        <v>69.02</v>
+      </c>
+      <c r="H19" s="10">
+        <v>70</v>
+      </c>
+      <c r="I19" s="10">
+        <v>71</v>
+      </c>
+      <c r="J19" s="10">
+        <v>72.099999999999994</v>
+      </c>
+      <c r="K19" s="10">
+        <v>73</v>
+      </c>
+      <c r="L19" s="10">
+        <v>74.5</v>
+      </c>
+      <c r="M19" s="10">
+        <v>75.599999999999994</v>
+      </c>
+      <c r="N19" s="10">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="O19" s="10">
+        <v>78.2</v>
+      </c>
+      <c r="P19" s="10">
+        <v>79.2</v>
+      </c>
+      <c r="Q19" s="10">
+        <v>80.099999999999994</v>
+      </c>
+      <c r="R19" s="10">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D20" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="10">
+        <v>1.43</v>
+      </c>
+      <c r="G20" s="10">
+        <v>1.48</v>
+      </c>
+      <c r="H20" s="10">
+        <v>1.52</v>
+      </c>
+      <c r="I20" s="10">
+        <v>1.6</v>
+      </c>
+      <c r="J20" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="K20" s="10">
+        <v>2.5</v>
+      </c>
+      <c r="L20" s="10">
+        <v>3</v>
+      </c>
+      <c r="M20" s="10">
+        <v>4.5</v>
+      </c>
+      <c r="N20" s="10">
+        <v>5</v>
+      </c>
+      <c r="O20" s="10">
+        <v>5</v>
+      </c>
+      <c r="P20" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>5</v>
+      </c>
+      <c r="R20" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="10">
+        <v>4.42</v>
+      </c>
+      <c r="G21" s="10">
+        <v>5.12</v>
+      </c>
+      <c r="H21" s="10">
+        <v>5.64</v>
+      </c>
+      <c r="I21" s="10">
+        <v>5.53</v>
+      </c>
+      <c r="J21" s="10">
+        <v>5.43</v>
+      </c>
+      <c r="K21" s="10">
+        <v>6.5</v>
+      </c>
+      <c r="L21" s="10">
+        <v>7.09</v>
+      </c>
+      <c r="M21" s="10">
+        <v>10.9</v>
+      </c>
+      <c r="N21" s="10">
+        <v>8.6</v>
+      </c>
+      <c r="O21" s="10">
+        <v>5.8</v>
+      </c>
+      <c r="P21" s="10">
+        <v>19.899999999999999</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>10.050000000000001</v>
+      </c>
+      <c r="R21" s="10">
+        <v>11.25</v>
+      </c>
+    </row>
+    <row r="22" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G22" s="8">
+        <v>0</v>
+      </c>
+      <c r="H22" s="8">
+        <v>0</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="J22" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="K22" s="8">
+        <v>0.87</v>
+      </c>
+      <c r="L22" s="8">
+        <v>6.8</v>
+      </c>
+      <c r="M22" s="8">
+        <v>6.03</v>
+      </c>
+      <c r="N22" s="8">
+        <v>3.38</v>
+      </c>
+      <c r="O22" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="P22" s="8">
+        <v>0.44</v>
+      </c>
+      <c r="Q22" s="8">
+        <v>0.51</v>
+      </c>
+      <c r="R22" s="8">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="23" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D23" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="8">
+        <v>10</v>
+      </c>
+      <c r="G23" s="8">
+        <v>12</v>
+      </c>
+      <c r="H23" s="8">
+        <v>13.43</v>
+      </c>
+      <c r="I23" s="8">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="J23" s="8">
+        <v>17</v>
+      </c>
+      <c r="K23" s="8">
+        <v>21</v>
+      </c>
+      <c r="L23" s="8">
+        <v>24.5</v>
+      </c>
+      <c r="M23" s="8">
+        <v>21</v>
+      </c>
+      <c r="N23" s="8">
+        <v>23</v>
+      </c>
+      <c r="O23" s="8">
+        <v>20</v>
+      </c>
+      <c r="P23" s="8">
+        <v>13.5</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>18</v>
+      </c>
+      <c r="R23" s="8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E24" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0</v>
+      </c>
+      <c r="G24" s="6">
+        <v>0</v>
+      </c>
+      <c r="H24" s="6">
+        <v>0</v>
+      </c>
+      <c r="I24" s="6">
+        <v>0</v>
+      </c>
+      <c r="J24" s="6">
+        <v>0</v>
+      </c>
+      <c r="K24" s="6">
+        <v>0</v>
+      </c>
+      <c r="L24" s="6">
+        <v>0</v>
+      </c>
+      <c r="M24" s="6">
+        <v>0</v>
+      </c>
+      <c r="N24" s="6">
+        <v>0</v>
+      </c>
+      <c r="O24" s="6">
+        <v>0</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="6">
+        <v>0</v>
+      </c>
+      <c r="R24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="4:18" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="4:18" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D26" s="19"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="20"/>
+      <c r="O26" s="20"/>
+      <c r="P26" s="20"/>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="20"/>
+    </row>
+    <row r="27" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D27" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="20"/>
+      <c r="N27" s="20"/>
+      <c r="O27" s="20"/>
+      <c r="P27" s="20"/>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="20"/>
+    </row>
+    <row r="28" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="20"/>
+      <c r="N28" s="20"/>
+      <c r="O28" s="20"/>
+      <c r="P28" s="20"/>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="20"/>
+    </row>
+    <row r="29" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="20"/>
+      <c r="O29" s="20"/>
+      <c r="P29" s="20"/>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="20"/>
+    </row>
+    <row r="30" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D30" s="7"/>
+      <c r="E30" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F30" s="8">
+        <v>6.66</v>
+      </c>
+      <c r="G30" s="8">
+        <v>1.82</v>
+      </c>
+      <c r="H30" s="8">
+        <v>0.02</v>
+      </c>
+      <c r="I30" s="8">
+        <v>0.17</v>
+      </c>
+      <c r="J30" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="K30" s="8">
+        <v>0</v>
+      </c>
+      <c r="L30" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="M30" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="N30" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="O30" s="8">
+        <v>0.41</v>
+      </c>
+      <c r="P30" s="8">
+        <v>6.13</v>
+      </c>
+      <c r="Q30" s="8">
+        <v>1.27</v>
+      </c>
+      <c r="R30" s="8">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="31" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D31" s="7"/>
+      <c r="E31" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="F31" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="G31" s="8">
+        <v>0</v>
+      </c>
+      <c r="H31" s="8">
+        <v>0.01</v>
+      </c>
+      <c r="I31" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="J31" s="8">
+        <v>0.06</v>
+      </c>
+      <c r="K31" s="8">
+        <v>1.71</v>
+      </c>
+      <c r="L31" s="8">
+        <v>8.65</v>
+      </c>
+      <c r="M31" s="8">
+        <v>5.37</v>
+      </c>
+      <c r="N31" s="8">
+        <v>1.67</v>
+      </c>
+      <c r="O31" s="8">
+        <v>0.81</v>
+      </c>
+      <c r="P31" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="Q31" s="8">
+        <v>0.45</v>
+      </c>
+      <c r="R31" s="8">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="32" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D32" s="22"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
+      <c r="Q32" s="23"/>
+      <c r="R32" s="23"/>
+    </row>
+    <row r="33" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D33" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="20"/>
+      <c r="G33" s="20"/>
+      <c r="H33" s="20"/>
+      <c r="I33" s="20"/>
+      <c r="J33" s="20"/>
+      <c r="K33" s="20"/>
+      <c r="L33" s="20"/>
+      <c r="M33" s="20"/>
+      <c r="N33" s="20"/>
+      <c r="O33" s="20"/>
+      <c r="P33" s="20"/>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="20"/>
+    </row>
+    <row r="34" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D34" s="2"/>
+      <c r="E34" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="20"/>
+      <c r="G34" s="20"/>
+      <c r="H34" s="20"/>
+      <c r="I34" s="20"/>
+      <c r="J34" s="20"/>
+      <c r="K34" s="20"/>
+      <c r="L34" s="20"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="20"/>
+      <c r="O34" s="20"/>
+      <c r="P34" s="20"/>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="20"/>
+    </row>
+    <row r="35" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D35" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="20"/>
+      <c r="J35" s="20"/>
+      <c r="K35" s="20"/>
+      <c r="L35" s="20"/>
+      <c r="M35" s="20"/>
+      <c r="N35" s="20"/>
+      <c r="O35" s="20"/>
+      <c r="P35" s="20"/>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="20"/>
+    </row>
+    <row r="36" spans="4:18" ht="28" x14ac:dyDescent="0.2">
+      <c r="D36" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="K36" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="L36" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N36" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="P36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q36" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="R36" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="37" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D37" s="7"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="14">
+        <v>1161978</v>
+      </c>
+      <c r="G37" s="14">
+        <v>1179681</v>
+      </c>
+      <c r="H37" s="14">
+        <v>1197147</v>
+      </c>
+      <c r="I37" s="14">
+        <v>1214270</v>
+      </c>
+      <c r="J37" s="14">
+        <v>1230981</v>
+      </c>
+      <c r="K37" s="14">
+        <v>1247236</v>
+      </c>
+      <c r="L37" s="14">
+        <v>1263066</v>
+      </c>
+      <c r="M37" s="14">
+        <v>1278562</v>
+      </c>
+      <c r="N37" s="14">
+        <v>1293859</v>
+      </c>
+      <c r="O37" s="14">
+        <v>1309054</v>
+      </c>
+      <c r="P37" s="14">
+        <v>1324171</v>
+      </c>
+      <c r="Q37" s="14">
+        <v>1339180</v>
+      </c>
+      <c r="R37" s="14">
+        <v>1354052</v>
+      </c>
+    </row>
+    <row r="38" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D38" s="7"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="8">
+        <v>58.7</v>
+      </c>
+      <c r="G38" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="H38" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="I38" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="J38" s="8">
+        <v>58.6</v>
+      </c>
+      <c r="K38" s="8">
+        <v>58.5</v>
+      </c>
+      <c r="L38" s="8">
+        <v>59</v>
+      </c>
+      <c r="M38" s="8">
+        <v>59.1</v>
+      </c>
+      <c r="N38" s="8">
+        <v>59.4</v>
+      </c>
+      <c r="O38" s="8">
+        <v>59.7</v>
+      </c>
+      <c r="P38" s="8">
+        <v>59.8</v>
+      </c>
+      <c r="Q38" s="8">
+        <v>59.8</v>
+      </c>
+      <c r="R38" s="8">
+        <v>59.8</v>
+      </c>
+    </row>
+    <row r="39" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D39" s="7"/>
+      <c r="E39" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="P39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q39" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="R39" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D40" s="7"/>
+      <c r="E40" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F40" s="8">
+        <v>26.48</v>
+      </c>
+      <c r="G40" s="8">
+        <v>27.99</v>
+      </c>
+      <c r="H40" s="8">
+        <v>28.04</v>
+      </c>
+      <c r="I40" s="8">
+        <v>27.75</v>
+      </c>
+      <c r="J40" s="8">
+        <v>28.46</v>
+      </c>
+      <c r="K40" s="8">
+        <v>29.07</v>
+      </c>
+      <c r="L40" s="8">
+        <v>29.86</v>
+      </c>
+      <c r="M40" s="8">
+        <v>29.65</v>
+      </c>
+      <c r="N40" s="8">
+        <v>30.47</v>
+      </c>
+      <c r="O40" s="8">
+        <v>31.47</v>
+      </c>
+      <c r="P40" s="8">
+        <v>30.23</v>
+      </c>
+      <c r="Q40" s="8">
+        <v>31.79</v>
+      </c>
+      <c r="R40" s="8">
+        <v>30.43</v>
+      </c>
+    </row>
+    <row r="41" spans="4:18" x14ac:dyDescent="0.2">
+      <c r="D41" s="7"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="8">
+        <v>2.62</v>
+      </c>
+      <c r="G41" s="8">
+        <v>2.71</v>
+      </c>
+      <c r="H41" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="I41" s="8">
+        <v>2.91</v>
+      </c>
+      <c r="J41" s="8">
+        <v>2.84</v>
+      </c>
+      <c r="K41" s="8">
+        <v>2.99</v>
+      </c>
+      <c r="L41" s="8">
+        <v>3.18</v>
+      </c>
+      <c r="M41" s="8">
+        <v>3.15</v>
+      </c>
+      <c r="N41" s="8">
+        <v>3.15</v>
+      </c>
+      <c r="O41" s="8">
+        <v>2.75</v>
+      </c>
+      <c r="P41" s="8">
+        <v>3.05</v>
+      </c>
+      <c r="Q41" s="8">
+        <v>3.1</v>
+      </c>
+      <c r="R41" s="8">
+        <v>3.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="E13:E24"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D32:R32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29247090-4910-F043-A63D-FDDD8732C11E}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="39.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
@@ -3528,7 +4890,7 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -3575,7 +4937,7 @@
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="8">
@@ -3622,7 +4984,7 @@
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="8">
@@ -3669,7 +5031,7 @@
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="8">
@@ -3716,7 +5078,7 @@
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -3763,7 +5125,7 @@
       <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="8">
@@ -3810,7 +5172,7 @@
       <c r="A16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="19" t="s">
+      <c r="B16" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="10">
@@ -3857,7 +5219,7 @@
       <c r="A17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="10">
@@ -3904,7 +5266,7 @@
       <c r="A18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="10">
@@ -3951,7 +5313,7 @@
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="8">
@@ -3998,7 +5360,7 @@
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="8">
@@ -4045,7 +5407,7 @@
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="18" t="s">
+      <c r="B21" s="23" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="6">
@@ -4108,23 +5470,23 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
@@ -4148,10 +5510,10 @@
       <c r="O24" s="16"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="23" t="s">
         <v>54</v>
       </c>
       <c r="C25" s="16"/>
@@ -4169,10 +5531,10 @@
       <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="18" t="s">
+      <c r="A26" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="16"/>
@@ -4193,7 +5555,7 @@
       <c r="A27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="8">
@@ -4240,7 +5602,7 @@
       <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="19" t="s">
+      <c r="B28" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="8">
@@ -4284,23 +5646,23 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="18"/>
-      <c r="C29" s="18"/>
-      <c r="D29" s="18"/>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
-      <c r="I29" s="18"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="18"/>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
-      <c r="N29" s="18"/>
-      <c r="O29" s="18"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
@@ -4649,12 +6011,1373 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A29:O29"/>
     <mergeCell ref="B10:B21"/>
     <mergeCell ref="A23:O23"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B27:B28"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76883C5F-835D-9748-BE94-2C4D2EBE429E}">
+  <dimension ref="A1:O38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17"/>
+      <c r="L3" s="17"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="17"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17"/>
+      <c r="O5" s="17"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17"/>
+      <c r="O6" s="17"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17"/>
+      <c r="O7" s="17"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+    </row>
+    <row r="9" spans="1:15" ht="28" x14ac:dyDescent="0.2">
+      <c r="A9" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L10" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="O10" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="8">
+        <v>3.55</v>
+      </c>
+      <c r="D11" s="8">
+        <v>3.45</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4.25</v>
+      </c>
+      <c r="F11" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="G11" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="H11" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="I11" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="J11" s="8">
+        <v>0.74</v>
+      </c>
+      <c r="K11" s="8">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="L11" s="8">
+        <v>5.8</v>
+      </c>
+      <c r="M11" s="8">
+        <v>2.11</v>
+      </c>
+      <c r="N11" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="O11" s="8">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="8">
+        <v>14.55</v>
+      </c>
+      <c r="D12" s="8">
+        <v>16.489999999999998</v>
+      </c>
+      <c r="E12" s="8">
+        <v>8.51</v>
+      </c>
+      <c r="F12" s="8">
+        <v>9.02</v>
+      </c>
+      <c r="G12" s="8">
+        <v>16.07</v>
+      </c>
+      <c r="H12" s="8">
+        <v>14.68</v>
+      </c>
+      <c r="I12" s="8">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="J12" s="8">
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="K12" s="8">
+        <v>13.93</v>
+      </c>
+      <c r="L12" s="8">
+        <v>11.3</v>
+      </c>
+      <c r="M12" s="8">
+        <v>18.399999999999999</v>
+      </c>
+      <c r="N12" s="8">
+        <v>18.5</v>
+      </c>
+      <c r="O12" s="8">
+        <v>19.46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8">
+        <v>0</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0</v>
+      </c>
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="8">
+        <v>0</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0</v>
+      </c>
+      <c r="J13" s="8">
+        <v>0</v>
+      </c>
+      <c r="K13" s="8">
+        <v>0</v>
+      </c>
+      <c r="L13" s="8">
+        <v>0</v>
+      </c>
+      <c r="M13" s="8">
+        <v>0</v>
+      </c>
+      <c r="N13" s="8">
+        <v>0</v>
+      </c>
+      <c r="O13" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="O14" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="8">
+        <v>4.92</v>
+      </c>
+      <c r="D15" s="8">
+        <v>5.07</v>
+      </c>
+      <c r="E15" s="8">
+        <v>5.04</v>
+      </c>
+      <c r="F15" s="8">
+        <v>5.15</v>
+      </c>
+      <c r="G15" s="8">
+        <v>5.45</v>
+      </c>
+      <c r="H15" s="8">
+        <v>5.4</v>
+      </c>
+      <c r="I15" s="8">
+        <v>5.15</v>
+      </c>
+      <c r="J15" s="8">
+        <v>5.57</v>
+      </c>
+      <c r="K15" s="8">
+        <v>5.7</v>
+      </c>
+      <c r="L15" s="8">
+        <v>5.73</v>
+      </c>
+      <c r="M15" s="8">
+        <v>5.69</v>
+      </c>
+      <c r="N15" s="8">
+        <v>5.79</v>
+      </c>
+      <c r="O15" s="8">
+        <v>5.81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="10">
+        <v>4.59</v>
+      </c>
+      <c r="D16" s="10">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E16" s="10">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="F16" s="10">
+        <v>4.75</v>
+      </c>
+      <c r="G16" s="10">
+        <v>4.8</v>
+      </c>
+      <c r="H16" s="10">
+        <v>4.8499999999999996</v>
+      </c>
+      <c r="I16" s="10">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="J16" s="10">
+        <v>5</v>
+      </c>
+      <c r="K16" s="10">
+        <v>5.05</v>
+      </c>
+      <c r="L16" s="10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="M16" s="10">
+        <v>5.15</v>
+      </c>
+      <c r="N16" s="10">
+        <v>5.21</v>
+      </c>
+      <c r="O16" s="10">
+        <v>5.26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0.37</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0.25</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0.13</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="N17" s="10">
+        <v>0.18</v>
+      </c>
+      <c r="O17" s="10">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A18" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.15</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0.2</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="M18" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="N18" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="O18" s="10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="8">
+        <v>9.73</v>
+      </c>
+      <c r="D19" s="8">
+        <v>10.62</v>
+      </c>
+      <c r="E19" s="8">
+        <v>6.32</v>
+      </c>
+      <c r="F19" s="8">
+        <v>4.2</v>
+      </c>
+      <c r="G19" s="8">
+        <v>8.39</v>
+      </c>
+      <c r="H19" s="8">
+        <v>11.53</v>
+      </c>
+      <c r="I19" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="J19" s="8">
+        <v>1.83</v>
+      </c>
+      <c r="K19" s="8">
+        <v>4.9800000000000004</v>
+      </c>
+      <c r="L19" s="8">
+        <v>9.27</v>
+      </c>
+      <c r="M19" s="8">
+        <v>13.52</v>
+      </c>
+      <c r="N19" s="8">
+        <v>12.47</v>
+      </c>
+      <c r="O19" s="8">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="8">
+        <v>3.45</v>
+      </c>
+      <c r="D20" s="8">
+        <v>4.25</v>
+      </c>
+      <c r="E20" s="8">
+        <v>1.4</v>
+      </c>
+      <c r="F20" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="G20" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1.06</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.74</v>
+      </c>
+      <c r="J20" s="8">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="K20" s="8">
+        <v>5.8</v>
+      </c>
+      <c r="L20" s="8">
+        <v>2.11</v>
+      </c>
+      <c r="M20" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="N20" s="8">
+        <v>1.55</v>
+      </c>
+      <c r="O20" s="8">
+        <v>1.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0</v>
+      </c>
+      <c r="E21" s="6">
+        <v>0</v>
+      </c>
+      <c r="F21" s="6">
+        <v>0</v>
+      </c>
+      <c r="G21" s="6">
+        <v>0</v>
+      </c>
+      <c r="H21" s="6">
+        <v>0</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0</v>
+      </c>
+      <c r="J21" s="6">
+        <v>0</v>
+      </c>
+      <c r="K21" s="6">
+        <v>0</v>
+      </c>
+      <c r="L21" s="6">
+        <v>0</v>
+      </c>
+      <c r="M21" s="6">
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
+        <v>0</v>
+      </c>
+      <c r="O21" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B22" s="17"/>
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="17"/>
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17"/>
+      <c r="F24" s="17"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="17"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="17"/>
+      <c r="O24" s="17"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="B25" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="17"/>
+      <c r="O25" s="17"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A26" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="17"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="17"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="17"/>
+      <c r="O26" s="17"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A27" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0</v>
+      </c>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+      <c r="E27" s="8">
+        <v>0</v>
+      </c>
+      <c r="F27" s="8">
+        <v>0</v>
+      </c>
+      <c r="G27" s="8">
+        <v>0</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0</v>
+      </c>
+      <c r="I27" s="8">
+        <v>0</v>
+      </c>
+      <c r="J27" s="8">
+        <v>0</v>
+      </c>
+      <c r="K27" s="8">
+        <v>0</v>
+      </c>
+      <c r="L27" s="8">
+        <v>0</v>
+      </c>
+      <c r="M27" s="8">
+        <v>0</v>
+      </c>
+      <c r="N27" s="8">
+        <v>0</v>
+      </c>
+      <c r="O27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A28" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="8">
+        <v>11.3</v>
+      </c>
+      <c r="D28" s="8">
+        <v>9.3699999999999992</v>
+      </c>
+      <c r="E28" s="8">
+        <v>8.1</v>
+      </c>
+      <c r="F28" s="8">
+        <v>5.23</v>
+      </c>
+      <c r="G28" s="8">
+        <v>7.61</v>
+      </c>
+      <c r="H28" s="8">
+        <v>11.86</v>
+      </c>
+      <c r="I28" s="8">
+        <v>7.23</v>
+      </c>
+      <c r="J28" s="8">
+        <v>1.33</v>
+      </c>
+      <c r="K28" s="8">
+        <v>3.82</v>
+      </c>
+      <c r="L28" s="8">
+        <v>8.42</v>
+      </c>
+      <c r="M28" s="8">
+        <v>11.97</v>
+      </c>
+      <c r="N28" s="8">
+        <v>13.72</v>
+      </c>
+      <c r="O28" s="8">
+        <v>13.72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A29" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A30" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" s="17"/>
+      <c r="D30" s="17"/>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="17"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="17"/>
+      <c r="O30" s="17"/>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="17"/>
+      <c r="D31" s="17"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="17"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="17"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="17"/>
+      <c r="O32" s="17"/>
+    </row>
+    <row r="33" spans="1:15" ht="28" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L33" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M33" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="N33" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="14">
+        <v>39559</v>
+      </c>
+      <c r="D34" s="14">
+        <v>39970</v>
+      </c>
+      <c r="E34" s="14">
+        <v>40382</v>
+      </c>
+      <c r="F34" s="14">
+        <v>40799</v>
+      </c>
+      <c r="G34" s="14">
+        <v>41224</v>
+      </c>
+      <c r="H34" s="14">
+        <v>41657</v>
+      </c>
+      <c r="I34" s="14">
+        <v>42097</v>
+      </c>
+      <c r="J34" s="14">
+        <v>42540</v>
+      </c>
+      <c r="K34" s="14">
+        <v>42982</v>
+      </c>
+      <c r="L34" s="14">
+        <v>43418</v>
+      </c>
+      <c r="M34" s="14">
+        <v>43847</v>
+      </c>
+      <c r="N34" s="14">
+        <v>44271</v>
+      </c>
+      <c r="O34" s="14">
+        <v>44689</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="C35" s="8">
+        <v>116</v>
+      </c>
+      <c r="D35" s="8">
+        <v>115.1</v>
+      </c>
+      <c r="E35" s="8">
+        <v>116.1</v>
+      </c>
+      <c r="F35" s="8">
+        <v>116.4</v>
+      </c>
+      <c r="G35" s="8">
+        <v>116.4</v>
+      </c>
+      <c r="H35" s="8">
+        <v>116.4</v>
+      </c>
+      <c r="I35" s="8">
+        <v>116.4</v>
+      </c>
+      <c r="J35" s="8">
+        <v>117.5</v>
+      </c>
+      <c r="K35" s="8">
+        <v>117.5</v>
+      </c>
+      <c r="L35" s="8">
+        <v>117.5</v>
+      </c>
+      <c r="M35" s="8">
+        <v>117.5</v>
+      </c>
+      <c r="N35" s="8">
+        <v>117.6</v>
+      </c>
+      <c r="O35" s="8">
+        <v>117.7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="I36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="K36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="L36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="O36" s="14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" s="8">
+        <v>5.54</v>
+      </c>
+      <c r="D37" s="8">
+        <v>5.83</v>
+      </c>
+      <c r="E37" s="8">
+        <v>4.34</v>
+      </c>
+      <c r="F37" s="8">
+        <v>3.24</v>
+      </c>
+      <c r="G37" s="8">
+        <v>4.58</v>
+      </c>
+      <c r="H37" s="8">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="I37" s="8">
+        <v>3.06</v>
+      </c>
+      <c r="J37" s="8">
+        <v>3.92</v>
+      </c>
+      <c r="K37" s="8">
+        <v>5.03</v>
+      </c>
+      <c r="L37" s="8">
+        <v>4.03</v>
+      </c>
+      <c r="M37" s="8">
+        <v>5.63</v>
+      </c>
+      <c r="N37" s="8">
+        <v>5.93</v>
+      </c>
+      <c r="O37" s="8">
+        <v>6.29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="C38" s="8">
+        <v>2.63</v>
+      </c>
+      <c r="D38" s="8">
+        <v>2.83</v>
+      </c>
+      <c r="E38" s="8">
+        <v>1.96</v>
+      </c>
+      <c r="F38" s="8">
+        <v>2.79</v>
+      </c>
+      <c r="G38" s="8">
+        <v>3.51</v>
+      </c>
+      <c r="H38" s="8">
+        <v>3.22</v>
+      </c>
+      <c r="I38" s="8">
+        <v>2.66</v>
+      </c>
+      <c r="J38" s="8">
+        <v>2.35</v>
+      </c>
+      <c r="K38" s="8">
+        <v>2.77</v>
+      </c>
+      <c r="L38" s="8">
+        <v>2.81</v>
+      </c>
+      <c r="M38" s="8">
+        <v>3.27</v>
+      </c>
+      <c r="N38" s="8">
+        <v>3.12</v>
+      </c>
+      <c r="O38" s="8">
+        <v>3.09</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
     <mergeCell ref="A29:O29"/>
+    <mergeCell ref="B10:B21"/>
+    <mergeCell ref="A23:O23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Abhinav | Create contraints between the variables in the same dimentions only
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/informationist/Projects/src/github.com/usc-isi-i2/sheet_annotator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A0B3EF9-EBB9-EA41-9989-067A6DF01BCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE0BEC5-FAAE-8B42-BE02-55BEA1DAD49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-4440" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" firstSheet="2" activeTab="7" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
   </bookViews>
   <sheets>
     <sheet name="india_wheat" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,10 @@
     <sheet name="shifted_india_wheat_wo_anchors" sheetId="6" r:id="rId3"/>
     <sheet name="usa_wheat" sheetId="4" r:id="rId4"/>
     <sheet name="argentina_wheat" sheetId="5" r:id="rId5"/>
+    <sheet name="e1" sheetId="7" r:id="rId6"/>
+    <sheet name="e1_shifted" sheetId="8" r:id="rId7"/>
+    <sheet name="e2" sheetId="9" r:id="rId8"/>
+    <sheet name="e2_shifted" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="103">
   <si>
     <t>Data Last Updated on:</t>
   </si>
@@ -338,6 +342,15 @@
   </si>
   <si>
     <t>For example, in the 2017/18 balance, the NMY refers to the crop that is harvested from November 2017 to January 2018 and marketed between December 2017 and November 2018</t>
+  </si>
+  <si>
+    <t>Heading 1</t>
+  </si>
+  <si>
+    <t>Heading 2</t>
+  </si>
+  <si>
+    <t>Heading 3</t>
   </si>
 </sst>
 </file>
@@ -2004,7 +2017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAEE078D-9750-1D4E-BA37-4A7256F92070}">
   <dimension ref="D4:R41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26:R26"/>
     </sheetView>
   </sheetViews>
@@ -7381,4 +7394,356 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C604983-1363-6A45-AC2B-CF50136EBD09}">
+  <dimension ref="I8:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="8" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I9">
+        <v>23</v>
+      </c>
+      <c r="J9">
+        <v>4</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>34</v>
+      </c>
+      <c r="J10">
+        <v>6</v>
+      </c>
+      <c r="K10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I11">
+        <v>45</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I12">
+        <v>56</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="9:11" x14ac:dyDescent="0.2">
+      <c r="I13">
+        <v>67</v>
+      </c>
+      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29D55BA8-8E2E-0542-9534-70C0D6154965}">
+  <dimension ref="C7:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>23</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>34</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <v>8</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>67</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1ED7A8-5599-D24C-874F-34E624EE6D8D}">
+  <dimension ref="B3:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>45</v>
+      </c>
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>56</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E2A8624-54D5-9944-9CF8-2825AC473B3E}">
+  <dimension ref="B4:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Abhinav | Add test case e3
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/informationist/Projects/src/github.com/usc-isi-i2/sheet_annotator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EE0BEC5-FAAE-8B42-BE02-55BEA1DAD49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55C7967-2BFC-0946-87A4-1EF54160E102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" firstSheet="2" activeTab="7" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" firstSheet="3" activeTab="9" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
   </bookViews>
   <sheets>
     <sheet name="india_wheat" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,8 @@
     <sheet name="e1_shifted" sheetId="8" r:id="rId7"/>
     <sheet name="e2" sheetId="9" r:id="rId8"/>
     <sheet name="e2_shifted" sheetId="10" r:id="rId9"/>
+    <sheet name="e3" sheetId="13" r:id="rId10"/>
+    <sheet name="e3_shifted" sheetId="14" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -42,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="104">
   <si>
     <t>Data Last Updated on:</t>
   </si>
@@ -351,6 +353,9 @@
   </si>
   <si>
     <t>Heading 3</t>
+  </si>
+  <si>
+    <t>Main subject</t>
   </si>
 </sst>
 </file>
@@ -847,8 +852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E291444-CA67-AD49-A6F4-57BDC8CB34D6}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2009,6 +2014,203 @@
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B27:B28"/>
   </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD91EDE-C5D0-A242-A296-3BA8250F47CB}">
+  <dimension ref="B3:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>34</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA50F8E-57F2-9D4E-9035-0A8FE34CBAA8}">
+  <dimension ref="C4:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" t="s">
+        <v>101</v>
+      </c>
+      <c r="E5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>23</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>34</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>45</v>
+      </c>
+      <c r="D9">
+        <v>8</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>56</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>67</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7401,7 +7603,7 @@
   <dimension ref="I8:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8:K13"/>
+      <selection activeCell="M33" sqref="M33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7568,8 +7770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F1ED7A8-5599-D24C-874F-34E624EE6D8D}">
   <dimension ref="B3:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:D9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7661,7 +7863,7 @@
   <dimension ref="B4:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B4" sqref="B4:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Abhinav | Improve constraint generation logic
* Create constraint only when overlapping in atleast one dimention
* This restriction doesn't apply on anchors
* Added more tests
* Create constraints only between variables in same dimention
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/informationist/Projects/src/github.com/usc-isi-i2/sheet_annotator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55C7967-2BFC-0946-87A4-1EF54160E102}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B30124-8F98-A240-845D-B312858C8CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" firstSheet="3" activeTab="9" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" firstSheet="6" activeTab="13" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
   </bookViews>
   <sheets>
     <sheet name="india_wheat" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,9 @@
     <sheet name="e2_shifted" sheetId="10" r:id="rId9"/>
     <sheet name="e3" sheetId="13" r:id="rId10"/>
     <sheet name="e3_shifted" sheetId="14" r:id="rId11"/>
+    <sheet name="e4" sheetId="15" r:id="rId12"/>
+    <sheet name="e4_shifted" sheetId="16" r:id="rId13"/>
+    <sheet name="e4_misaligned" sheetId="17" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -44,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="109">
   <si>
     <t>Data Last Updated on:</t>
   </si>
@@ -356,6 +359,21 @@
   </si>
   <si>
     <t>Main subject</t>
+  </si>
+  <si>
+    <t>Column 1</t>
+  </si>
+  <si>
+    <t>Column 2</t>
+  </si>
+  <si>
+    <t>Column 3</t>
+  </si>
+  <si>
+    <t>anchor 1</t>
+  </si>
+  <si>
+    <t>Column 4</t>
   </si>
 </sst>
 </file>
@@ -852,8 +870,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E291444-CA67-AD49-A6F4-57BDC8CB34D6}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2022,7 +2040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD91EDE-C5D0-A242-A296-3BA8250F47CB}">
   <dimension ref="B3:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2123,7 +2141,7 @@
   <dimension ref="C4:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2208,6 +2226,522 @@
       </c>
       <c r="E11">
         <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C890DECD-018C-2F45-AB56-F4507EE6E86D}">
+  <dimension ref="B3:E16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>45</v>
+      </c>
+      <c r="D8">
+        <v>8</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>56</v>
+      </c>
+      <c r="D9">
+        <v>10</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>67</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>8</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="D16">
+        <v>10</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C76F06-1848-654B-A330-D2315B33BA4B}">
+  <dimension ref="C4:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>56</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>67</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>3</v>
+      </c>
+      <c r="E15">
+        <v>6</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>10</v>
+      </c>
+      <c r="F17">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F81CEF8-CDBD-504E-B962-415A53D098DD}">
+  <dimension ref="C4:I17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>23</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>34</v>
+      </c>
+      <c r="E8">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>45</v>
+      </c>
+      <c r="E9">
+        <v>8</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>56</v>
+      </c>
+      <c r="E10">
+        <v>10</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>67</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>107</v>
+      </c>
+      <c r="F12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" t="s">
+        <v>106</v>
+      </c>
+      <c r="I12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <v>6</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>6</v>
+      </c>
+      <c r="H15">
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>4</v>
+      </c>
+      <c r="G16">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>12</v>
+      </c>
+      <c r="I16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="6:9" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>5</v>
+      </c>
+      <c r="G17">
+        <v>10</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="I17">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3580,11 +4114,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B5EE06-08CE-BF4A-884D-58CF4ACB1707}">
   <dimension ref="D4:R41"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="4" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D4" s="1"/>
@@ -3625,7 +4163,9 @@
       <c r="R5" s="20"/>
     </row>
     <row r="6" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="E6" s="2" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Abhinav | Ignore empty rows/columns for annotation transfer
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/informationist/Projects/src/github.com/usc-isi-i2/sheet_annotator/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8B30124-8F98-A240-845D-B312858C8CE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439AA394-7389-364F-927F-7B43A8380F44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20480" windowHeight="12800" firstSheet="6" activeTab="13" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
+    <workbookView xWindow="-21600" yWindow="0" windowWidth="21600" windowHeight="16200" firstSheet="7" activeTab="15" xr2:uid="{166A31F6-BC75-F342-9533-F37DF65F07D0}"/>
   </bookViews>
   <sheets>
     <sheet name="india_wheat" sheetId="1" r:id="rId1"/>
@@ -22,11 +22,14 @@
     <sheet name="e1_shifted" sheetId="8" r:id="rId7"/>
     <sheet name="e2" sheetId="9" r:id="rId8"/>
     <sheet name="e2_shifted" sheetId="10" r:id="rId9"/>
-    <sheet name="e3" sheetId="13" r:id="rId10"/>
-    <sheet name="e3_shifted" sheetId="14" r:id="rId11"/>
-    <sheet name="e4" sheetId="15" r:id="rId12"/>
-    <sheet name="e4_shifted" sheetId="16" r:id="rId13"/>
-    <sheet name="e4_misaligned" sheetId="17" r:id="rId14"/>
+    <sheet name="Sheet2" sheetId="19" r:id="rId10"/>
+    <sheet name="e3" sheetId="13" r:id="rId11"/>
+    <sheet name="e3_shifted" sheetId="14" r:id="rId12"/>
+    <sheet name="e4" sheetId="15" r:id="rId13"/>
+    <sheet name="e4_shifted" sheetId="16" r:id="rId14"/>
+    <sheet name="e4_misaligned" sheetId="17" r:id="rId15"/>
+    <sheet name="e4_empty_row" sheetId="18" r:id="rId16"/>
+    <sheet name="e2_empty_row" sheetId="20" r:id="rId17"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -47,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="706" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="109">
   <si>
     <t>Data Last Updated on:</t>
   </si>
@@ -493,7 +496,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -542,6 +545,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -871,7 +877,7 @@
   <dimension ref="A1:O38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -996,7 +1002,7 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -1043,7 +1049,7 @@
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="8">
@@ -1090,7 +1096,7 @@
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="8">
@@ -1137,7 +1143,7 @@
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="8">
@@ -1184,7 +1190,7 @@
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -1231,7 +1237,7 @@
       <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="8">
@@ -1278,7 +1284,7 @@
       <c r="A16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="10">
@@ -1325,7 +1331,7 @@
       <c r="A17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="10">
@@ -1372,7 +1378,7 @@
       <c r="A18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="10">
@@ -1419,7 +1425,7 @@
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="8">
@@ -1466,7 +1472,7 @@
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="8">
@@ -1513,7 +1519,7 @@
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="6">
@@ -1562,23 +1568,23 @@
       </c>
     </row>
     <row r="23" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
@@ -1589,18 +1595,18 @@
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="24" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="23" t="s">
+      <c r="A26" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1608,7 +1614,7 @@
       <c r="A27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="8">
@@ -1655,7 +1661,7 @@
       <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="8">
@@ -1699,23 +1705,23 @@
       </c>
     </row>
     <row r="29" spans="1:15" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
@@ -2037,6 +2043,18 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDA7E98-2C80-5741-9B9C-D2D1E59E70EF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DD91EDE-C5D0-A242-A296-3BA8250F47CB}">
   <dimension ref="B3:D10"/>
   <sheetViews>
@@ -2136,7 +2154,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA50F8E-57F2-9D4E-9035-0A8FE34CBAA8}">
   <dimension ref="C4:E11"/>
   <sheetViews>
@@ -2233,12 +2251,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C890DECD-018C-2F45-AB56-F4507EE6E86D}">
   <dimension ref="B3:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D13" sqref="B3:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2399,7 +2417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93C76F06-1848-654B-A330-D2315B33BA4B}">
   <dimension ref="C4:F17"/>
   <sheetViews>
@@ -2565,12 +2583,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F81CEF8-CDBD-504E-B962-415A53D098DD}">
   <dimension ref="C4:I17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2742,6 +2760,198 @@
       </c>
       <c r="I17">
         <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E074476-DC7F-F049-A07C-6D54A8BD22A6}">
+  <dimension ref="B3:E16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>100</v>
+      </c>
+      <c r="E4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>23</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>45</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>56</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>67</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>5</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A06AB28E-445B-5B44-840F-AB7294688C69}">
+  <dimension ref="B4:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>23</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>45</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>56</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>67</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2978,7 +3188,7 @@
       <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -3025,7 +3235,7 @@
       <c r="D14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="8">
@@ -3072,7 +3282,7 @@
       <c r="D15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="8">
@@ -3119,7 +3329,7 @@
       <c r="D16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="8">
@@ -3166,7 +3376,7 @@
       <c r="D17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -3213,7 +3423,7 @@
       <c r="D18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="8">
@@ -3260,7 +3470,7 @@
       <c r="D19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="10">
@@ -3307,7 +3517,7 @@
       <c r="D20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="10">
@@ -3354,7 +3564,7 @@
       <c r="D21" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="10">
@@ -3401,7 +3611,7 @@
       <c r="D22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="8">
@@ -3448,7 +3658,7 @@
       <c r="D23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F23" s="8">
@@ -3495,7 +3705,7 @@
       <c r="D24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="26" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="6">
@@ -3558,23 +3768,23 @@
       <c r="R25" s="12"/>
     </row>
     <row r="26" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-      <c r="K26" s="23"/>
-      <c r="L26" s="23"/>
-      <c r="M26" s="23"/>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
+      <c r="Q26" s="24"/>
+      <c r="R26" s="24"/>
     </row>
     <row r="27" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D27" s="12" t="s">
@@ -3598,10 +3808,10 @@
       <c r="R27" s="12"/>
     </row>
     <row r="28" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D28" s="23" t="s">
+      <c r="D28" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="24" t="s">
         <v>54</v>
       </c>
       <c r="F28" s="12"/>
@@ -3619,10 +3829,10 @@
       <c r="R28" s="12"/>
     </row>
     <row r="29" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D29" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="23" t="s">
+      <c r="D29" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="24" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="12"/>
@@ -3643,7 +3853,7 @@
       <c r="D30" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F30" s="8">
@@ -3690,7 +3900,7 @@
       <c r="D31" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="8">
@@ -3734,23 +3944,23 @@
       </c>
     </row>
     <row r="32" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
     </row>
     <row r="33" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D33" s="12" t="s">
@@ -4114,8 +4324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0B5EE06-08CE-BF4A-884D-58CF4ACB1707}">
   <dimension ref="D4:R41"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4205,12 +4415,8 @@
       <c r="R7" s="20"/>
     </row>
     <row r="8" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D8" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
@@ -4226,12 +4432,8 @@
       <c r="R8" s="20"/>
     </row>
     <row r="9" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D9" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
@@ -4247,10 +4449,10 @@
       <c r="R9" s="20"/>
     </row>
     <row r="10" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D10" s="2"/>
-      <c r="E10" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="20"/>
       <c r="F10" s="20"/>
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
@@ -4266,12 +4468,8 @@
       <c r="R10" s="20"/>
     </row>
     <row r="11" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D11" s="20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>8</v>
-      </c>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
       <c r="F11" s="20"/>
       <c r="G11" s="20"/>
       <c r="H11" s="20"/>
@@ -4287,8 +4485,12 @@
       <c r="R11" s="20"/>
     </row>
     <row r="12" spans="4:18" ht="28" x14ac:dyDescent="0.2">
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
+      <c r="D12" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>11</v>
+      </c>
       <c r="F12" s="4" t="s">
         <v>12</v>
       </c>
@@ -4333,7 +4535,7 @@
       <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F13" s="6" t="s">
@@ -4380,7 +4582,7 @@
       <c r="D14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F14" s="8">
@@ -4427,7 +4629,7 @@
       <c r="D15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F15" s="8">
@@ -4474,7 +4676,7 @@
       <c r="D16" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F16" s="8">
@@ -4521,7 +4723,7 @@
       <c r="D17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -4568,7 +4770,7 @@
       <c r="D18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F18" s="8">
@@ -4615,7 +4817,7 @@
       <c r="D19" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="10">
@@ -4662,7 +4864,7 @@
       <c r="D20" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F20" s="10">
@@ -4709,7 +4911,7 @@
       <c r="D21" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="10">
@@ -4756,7 +4958,7 @@
       <c r="D22" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F22" s="8">
@@ -4803,7 +5005,7 @@
       <c r="D23" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F23" s="8">
@@ -4850,7 +5052,7 @@
       <c r="D24" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E24" s="25" t="s">
+      <c r="E24" s="26" t="s">
         <v>26</v>
       </c>
       <c r="F24" s="6">
@@ -4933,8 +5135,8 @@
       <c r="R27" s="20"/>
     </row>
     <row r="28" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
       <c r="F28" s="20"/>
       <c r="G28" s="20"/>
       <c r="H28" s="20"/>
@@ -4950,8 +5152,8 @@
       <c r="R28" s="20"/>
     </row>
     <row r="29" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
       <c r="F29" s="20"/>
       <c r="G29" s="20"/>
       <c r="H29" s="20"/>
@@ -4968,7 +5170,7 @@
     </row>
     <row r="30" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D30" s="7"/>
-      <c r="E30" s="24" t="s">
+      <c r="E30" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F30" s="8">
@@ -5013,7 +5215,7 @@
     </row>
     <row r="31" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D31" s="7"/>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="25" t="s">
         <v>26</v>
       </c>
       <c r="F31" s="8">
@@ -5057,21 +5259,21 @@
       </c>
     </row>
     <row r="32" spans="4:18" x14ac:dyDescent="0.2">
-      <c r="D32" s="22"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-      <c r="K32" s="23"/>
-      <c r="L32" s="23"/>
-      <c r="M32" s="23"/>
-      <c r="N32" s="23"/>
-      <c r="O32" s="23"/>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="23"/>
-      <c r="R32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="24"/>
+      <c r="F32" s="24"/>
+      <c r="G32" s="24"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
+      <c r="K32" s="24"/>
+      <c r="L32" s="24"/>
+      <c r="M32" s="24"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
+      <c r="P32" s="24"/>
+      <c r="Q32" s="24"/>
+      <c r="R32" s="24"/>
     </row>
     <row r="33" spans="4:18" x14ac:dyDescent="0.2">
       <c r="D33" s="20" t="s">
@@ -5645,7 +5847,7 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -5692,7 +5894,7 @@
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="8">
@@ -5739,7 +5941,7 @@
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="8">
@@ -5786,7 +5988,7 @@
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="8">
@@ -5833,7 +6035,7 @@
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -5880,7 +6082,7 @@
       <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="8">
@@ -5927,7 +6129,7 @@
       <c r="A16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="10">
@@ -5974,7 +6176,7 @@
       <c r="A17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="10">
@@ -6021,7 +6223,7 @@
       <c r="A18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="10">
@@ -6068,7 +6270,7 @@
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="8">
@@ -6115,7 +6317,7 @@
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="8">
@@ -6162,7 +6364,7 @@
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="24" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="6">
@@ -6225,23 +6427,23 @@
       <c r="O22" s="16"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
@@ -6265,10 +6467,10 @@
       <c r="O24" s="16"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="24" t="s">
         <v>54</v>
       </c>
       <c r="C25" s="16"/>
@@ -6286,10 +6488,10 @@
       <c r="O25" s="16"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="23" t="s">
+      <c r="A26" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="16"/>
@@ -6310,7 +6512,7 @@
       <c r="A27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="8">
@@ -6357,7 +6559,7 @@
       <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="8">
@@ -6401,23 +6603,23 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
@@ -7006,7 +7208,7 @@
       <c r="A10" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="6" t="s">
@@ -7053,7 +7255,7 @@
       <c r="A11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="8">
@@ -7100,7 +7302,7 @@
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="8">
@@ -7147,7 +7349,7 @@
       <c r="A13" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C13" s="8">
@@ -7194,7 +7396,7 @@
       <c r="A14" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="6" t="s">
@@ -7241,7 +7443,7 @@
       <c r="A15" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C15" s="8">
@@ -7288,7 +7490,7 @@
       <c r="A16" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="24" t="s">
+      <c r="B16" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C16" s="10">
@@ -7335,7 +7537,7 @@
       <c r="A17" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="24" t="s">
+      <c r="B17" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C17" s="10">
@@ -7382,7 +7584,7 @@
       <c r="A18" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B18" s="24" t="s">
+      <c r="B18" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C18" s="10">
@@ -7429,7 +7631,7 @@
       <c r="A19" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B19" s="24" t="s">
+      <c r="B19" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C19" s="8">
@@ -7476,7 +7678,7 @@
       <c r="A20" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C20" s="8">
@@ -7523,7 +7725,7 @@
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="26" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="6">
@@ -7586,23 +7788,23 @@
       <c r="O22" s="17"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="22" t="s">
+      <c r="A23" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-      <c r="K23" s="23"/>
-      <c r="L23" s="23"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="24"/>
+      <c r="G23" s="24"/>
+      <c r="H23" s="24"/>
+      <c r="I23" s="24"/>
+      <c r="J23" s="24"/>
+      <c r="K23" s="24"/>
+      <c r="L23" s="24"/>
+      <c r="M23" s="24"/>
+      <c r="N23" s="24"/>
+      <c r="O23" s="24"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" s="17" t="s">
@@ -7626,10 +7828,10 @@
       <c r="O24" s="17"/>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="23" t="s">
+      <c r="A25" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="24" t="s">
         <v>54</v>
       </c>
       <c r="C25" s="17"/>
@@ -7647,10 +7849,10 @@
       <c r="O25" s="17"/>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B26" s="23" t="s">
+      <c r="A26" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" s="24" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="17"/>
@@ -7671,7 +7873,7 @@
       <c r="A27" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B27" s="24" t="s">
+      <c r="B27" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C27" s="8">
@@ -7718,7 +7920,7 @@
       <c r="A28" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="B28" s="24" t="s">
+      <c r="B28" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C28" s="8">
@@ -7762,23 +7964,23 @@
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="22" t="s">
+      <c r="A29" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-      <c r="K29" s="23"/>
-      <c r="L29" s="23"/>
-      <c r="M29" s="23"/>
-      <c r="N29" s="23"/>
-      <c r="O29" s="23"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
+      <c r="F29" s="24"/>
+      <c r="G29" s="24"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
+      <c r="K29" s="24"/>
+      <c r="L29" s="24"/>
+      <c r="M29" s="24"/>
+      <c r="N29" s="24"/>
+      <c r="O29" s="24"/>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A30" s="17" t="s">
@@ -8143,7 +8345,7 @@
   <dimension ref="I8:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M33" sqref="M33"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>